<commit_message>
started work on nest automation
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -638,7 +638,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,22 +673,22 @@
         <v>6</v>
       </c>
       <c r="B2" s="8">
-        <v>2714.95</v>
+        <v>2612.4499999999998</v>
       </c>
       <c r="C2" s="11">
-        <v>2668.2</v>
+        <v>2531.1</v>
       </c>
       <c r="D2" s="14">
-        <v>2694.9</v>
+        <v>2542.1999999999998</v>
       </c>
       <c r="E2" s="5">
-        <v>2698.05</v>
+        <v>2539.5500000000002</v>
       </c>
       <c r="F2" s="17">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="G2" s="5">
-        <v>2705.95</v>
+        <v>2571.65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -696,22 +696,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="9">
-        <v>401.5</v>
+        <v>399.55</v>
       </c>
       <c r="C3" s="12">
-        <v>392.05</v>
+        <v>393.1</v>
       </c>
       <c r="D3" s="15">
-        <v>393.85</v>
+        <v>394.7</v>
       </c>
       <c r="E3" s="6">
-        <v>393.95</v>
+        <v>395.6</v>
       </c>
       <c r="F3" s="18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="6">
-        <v>398.6</v>
+        <v>397.5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -719,22 +719,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="9">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="C4" s="12">
-        <v>1464.35</v>
+        <v>1465</v>
       </c>
       <c r="D4" s="15">
-        <v>1468.5</v>
+        <v>1467</v>
       </c>
       <c r="E4" s="6">
-        <v>1467.8</v>
+        <v>1468.6</v>
       </c>
       <c r="F4" s="18">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G4" s="6">
-        <v>1482</v>
+        <v>1489.2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -742,22 +742,22 @@
         <v>9</v>
       </c>
       <c r="B5" s="9">
-        <v>7153.5</v>
+        <v>7185.95</v>
       </c>
       <c r="C5" s="12">
-        <v>7050</v>
+        <v>7121</v>
       </c>
       <c r="D5" s="15">
-        <v>7053.25</v>
+        <v>7124</v>
       </c>
       <c r="E5" s="6">
-        <v>7069.95</v>
+        <v>7137.45</v>
       </c>
       <c r="F5" s="18">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G5" s="6">
-        <v>7056.05</v>
+        <v>7179</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -765,22 +765,22 @@
         <v>10</v>
       </c>
       <c r="B6" s="9">
-        <v>232.7</v>
+        <v>240.7</v>
       </c>
       <c r="C6" s="12">
-        <v>230.8</v>
+        <v>234</v>
       </c>
       <c r="D6" s="15">
-        <v>231.95</v>
+        <v>235.2</v>
       </c>
       <c r="E6" s="6">
-        <v>232.1</v>
+        <v>234.9</v>
       </c>
       <c r="F6" s="18">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="G6" s="6">
-        <v>231.8</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -788,22 +788,22 @@
         <v>11</v>
       </c>
       <c r="B7" s="9">
-        <v>191.8</v>
+        <v>194.95</v>
       </c>
       <c r="C7" s="12">
-        <v>189.85</v>
+        <v>190.75</v>
       </c>
       <c r="D7" s="15">
-        <v>190.3</v>
+        <v>191.9</v>
       </c>
       <c r="E7" s="6">
-        <v>190.25</v>
+        <v>191.85</v>
       </c>
       <c r="F7" s="18">
-        <v>108</v>
+        <v>159</v>
       </c>
       <c r="G7" s="6">
-        <v>191.45</v>
+        <v>194.55</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -811,22 +811,22 @@
         <v>12</v>
       </c>
       <c r="B8" s="9">
-        <v>232.05</v>
+        <v>232.65</v>
       </c>
       <c r="C8" s="12">
-        <v>229.7</v>
+        <v>228.5</v>
       </c>
       <c r="D8" s="15">
-        <v>230.85</v>
+        <v>229.75</v>
       </c>
       <c r="E8" s="6">
-        <v>230.75</v>
+        <v>229.25</v>
       </c>
       <c r="F8" s="18">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G8" s="6">
-        <v>230.15</v>
+        <v>232.3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -834,22 +834,22 @@
         <v>13</v>
       </c>
       <c r="B9" s="9">
+        <v>490.75</v>
+      </c>
+      <c r="C9" s="12">
+        <v>483</v>
+      </c>
+      <c r="D9" s="15">
+        <v>483.5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>483.55</v>
+      </c>
+      <c r="F9" s="18">
+        <v>26</v>
+      </c>
+      <c r="G9" s="6">
         <v>484.85</v>
-      </c>
-      <c r="C9" s="12">
-        <v>479.55</v>
-      </c>
-      <c r="D9" s="15">
-        <v>480</v>
-      </c>
-      <c r="E9" s="6">
-        <v>480.35</v>
-      </c>
-      <c r="F9" s="18">
-        <v>15</v>
-      </c>
-      <c r="G9" s="6">
-        <v>481.9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -857,22 +857,22 @@
         <v>14</v>
       </c>
       <c r="B10" s="9">
-        <v>3369</v>
+        <v>3367.7</v>
       </c>
       <c r="C10" s="12">
-        <v>3329</v>
+        <v>3320</v>
       </c>
       <c r="D10" s="15">
-        <v>3338</v>
+        <v>3325</v>
       </c>
       <c r="E10" s="6">
-        <v>3343.4</v>
+        <v>3341.65</v>
       </c>
       <c r="F10" s="18">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G10" s="6">
-        <v>3364</v>
+        <v>3353</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -880,22 +880,22 @@
         <v>15</v>
       </c>
       <c r="B11" s="9">
-        <v>136.9</v>
+        <v>143.15</v>
       </c>
       <c r="C11" s="12">
-        <v>134.1</v>
+        <v>139.4</v>
       </c>
       <c r="D11" s="15">
-        <v>135.80000000000001</v>
+        <v>140.6</v>
       </c>
       <c r="E11" s="6">
-        <v>136.05000000000001</v>
+        <v>140.69999999999999</v>
       </c>
       <c r="F11" s="18">
-        <v>156</v>
+        <v>226</v>
       </c>
       <c r="G11" s="6">
-        <v>134.5</v>
+        <v>142.80000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -903,22 +903,22 @@
         <v>16</v>
       </c>
       <c r="B12" s="9">
-        <v>1186</v>
+        <v>1188.8</v>
       </c>
       <c r="C12" s="12">
-        <v>1176.1500000000001</v>
+        <v>1169</v>
       </c>
       <c r="D12" s="15">
-        <v>1180</v>
+        <v>1172.95</v>
       </c>
       <c r="E12" s="6">
-        <v>1179.5</v>
+        <v>1171.25</v>
       </c>
       <c r="F12" s="18">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G12" s="6">
-        <v>1185.95</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -926,22 +926,22 @@
         <v>17</v>
       </c>
       <c r="B13" s="9">
-        <v>1595.95</v>
+        <v>1596.2</v>
       </c>
       <c r="C13" s="12">
-        <v>1580</v>
+        <v>1576.15</v>
       </c>
       <c r="D13" s="15">
-        <v>1581.45</v>
+        <v>1579.6</v>
       </c>
       <c r="E13" s="6">
-        <v>1582.7</v>
+        <v>1579.3</v>
       </c>
       <c r="F13" s="18">
-        <v>161</v>
+        <v>215</v>
       </c>
       <c r="G13" s="6">
-        <v>1593.05</v>
+        <v>1591.05</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -949,22 +949,22 @@
         <v>18</v>
       </c>
       <c r="B14" s="9">
-        <v>454.4</v>
+        <v>464.65</v>
       </c>
       <c r="C14" s="12">
-        <v>448.8</v>
+        <v>453.85</v>
       </c>
       <c r="D14" s="15">
-        <v>451</v>
+        <v>455.55</v>
       </c>
       <c r="E14" s="6">
-        <v>450.35</v>
+        <v>456.5</v>
       </c>
       <c r="F14" s="18">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="G14" s="6">
-        <v>451.85</v>
+        <v>464.4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,22 +972,22 @@
         <v>19</v>
       </c>
       <c r="B15" s="9">
-        <v>956.65</v>
+        <v>982.4</v>
       </c>
       <c r="C15" s="12">
-        <v>949.3</v>
+        <v>966.75</v>
       </c>
       <c r="D15" s="15">
-        <v>950</v>
+        <v>968.8</v>
       </c>
       <c r="E15" s="6">
-        <v>952</v>
+        <v>968.95</v>
       </c>
       <c r="F15" s="18">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="G15" s="6">
-        <v>953.7</v>
+        <v>974.3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -995,22 +995,22 @@
         <v>20</v>
       </c>
       <c r="B16" s="9">
-        <v>1404</v>
+        <v>1435</v>
       </c>
       <c r="C16" s="12">
-        <v>1394.1</v>
+        <v>1411.95</v>
       </c>
       <c r="D16" s="15">
-        <v>1397.8</v>
+        <v>1418.65</v>
       </c>
       <c r="E16" s="6">
-        <v>1401.15</v>
+        <v>1425.15</v>
       </c>
       <c r="F16" s="18">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="G16" s="6">
-        <v>1397.05</v>
+        <v>1414.15</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1018,22 +1018,22 @@
         <v>21</v>
       </c>
       <c r="B17" s="9">
-        <v>1405.95</v>
+        <v>1425.05</v>
       </c>
       <c r="C17" s="12">
-        <v>1396.65</v>
+        <v>1414.45</v>
       </c>
       <c r="D17" s="15">
-        <v>1404</v>
+        <v>1424</v>
       </c>
       <c r="E17" s="6">
-        <v>1403.75</v>
+        <v>1423.6</v>
       </c>
       <c r="F17" s="18">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="G17" s="6">
-        <v>1402.65</v>
+        <v>1419.75</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1041,22 +1041,22 @@
         <v>22</v>
       </c>
       <c r="B18" s="9">
-        <v>658.7</v>
+        <v>667.5</v>
       </c>
       <c r="C18" s="12">
-        <v>649.25</v>
+        <v>647</v>
       </c>
       <c r="D18" s="15">
-        <v>654.4</v>
+        <v>647.70000000000005</v>
       </c>
       <c r="E18" s="6">
-        <v>655.85</v>
+        <v>649.1</v>
       </c>
       <c r="F18" s="18">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G18" s="6">
-        <v>656.15</v>
+        <v>664.3</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1064,22 +1064,22 @@
         <v>23</v>
       </c>
       <c r="B19" s="9">
-        <v>427.15</v>
+        <v>426.1</v>
       </c>
       <c r="C19" s="12">
-        <v>421.5</v>
+        <v>419.9</v>
       </c>
       <c r="D19" s="15">
-        <v>423</v>
+        <v>420.45</v>
       </c>
       <c r="E19" s="6">
-        <v>422.9</v>
+        <v>421.55</v>
       </c>
       <c r="F19" s="18">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G19" s="6">
-        <v>421.6</v>
+        <v>425.95</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1087,22 +1087,22 @@
         <v>24</v>
       </c>
       <c r="B20" s="9">
-        <v>1555</v>
+        <v>1553.3</v>
       </c>
       <c r="C20" s="12">
-        <v>1541</v>
+        <v>1528.05</v>
       </c>
       <c r="D20" s="15">
-        <v>1550</v>
+        <v>1542</v>
       </c>
       <c r="E20" s="6">
-        <v>1550.5</v>
+        <v>1542.2</v>
       </c>
       <c r="F20" s="18">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G20" s="6">
-        <v>1547.3</v>
+        <v>1550.9</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1110,22 +1110,22 @@
         <v>25</v>
       </c>
       <c r="B21" s="9">
-        <v>289.60000000000002</v>
+        <v>306</v>
       </c>
       <c r="C21" s="12">
-        <v>276.5</v>
+        <v>299</v>
       </c>
       <c r="D21" s="15">
-        <v>288.7</v>
+        <v>304.3</v>
       </c>
       <c r="E21" s="6">
-        <v>288.64999999999998</v>
+        <v>304.05</v>
       </c>
       <c r="F21" s="18">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G21" s="6">
-        <v>277</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1133,22 +1133,22 @@
         <v>26</v>
       </c>
       <c r="B22" s="9">
-        <v>2537.9499999999998</v>
+        <v>2539</v>
       </c>
       <c r="C22" s="12">
-        <v>2507</v>
+        <v>2471</v>
       </c>
       <c r="D22" s="15">
-        <v>2523</v>
+        <v>2475.8000000000002</v>
       </c>
       <c r="E22" s="6">
-        <v>2519.4</v>
+        <v>2479.8000000000002</v>
       </c>
       <c r="F22" s="18">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="G22" s="6">
-        <v>2509.3000000000002</v>
+        <v>2529.4</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1156,22 +1156,22 @@
         <v>27</v>
       </c>
       <c r="B23" s="9">
-        <v>574.45000000000005</v>
+        <v>582</v>
       </c>
       <c r="C23" s="12">
-        <v>567.5</v>
+        <v>575.54999999999995</v>
       </c>
       <c r="D23" s="15">
-        <v>568.20000000000005</v>
+        <v>577</v>
       </c>
       <c r="E23" s="6">
-        <v>568.5</v>
+        <v>576.95000000000005</v>
       </c>
       <c r="F23" s="18">
-        <v>140</v>
+        <v>241</v>
       </c>
       <c r="G23" s="6">
-        <v>572.54999999999995</v>
+        <v>580.35</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1179,22 +1179,22 @@
         <v>28</v>
       </c>
       <c r="B24" s="9">
-        <v>548.5</v>
+        <v>585.9</v>
       </c>
       <c r="C24" s="12">
-        <v>539.1</v>
+        <v>566.04999999999995</v>
       </c>
       <c r="D24" s="15">
-        <v>541</v>
+        <v>582.70000000000005</v>
       </c>
       <c r="E24" s="6">
-        <v>542</v>
+        <v>582.54999999999995</v>
       </c>
       <c r="F24" s="18">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="G24" s="6">
-        <v>544.5</v>
+        <v>571.1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1202,22 +1202,22 @@
         <v>29</v>
       </c>
       <c r="B25" s="9">
-        <v>1008</v>
+        <v>1017.4</v>
       </c>
       <c r="C25" s="12">
-        <v>1000.3</v>
+        <v>1004.15</v>
       </c>
       <c r="D25" s="15">
-        <v>1004.9</v>
+        <v>1017</v>
       </c>
       <c r="E25" s="6">
-        <v>1004</v>
+        <v>1015.65</v>
       </c>
       <c r="F25" s="18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G25" s="6">
-        <v>1002.55</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1225,22 +1225,22 @@
         <v>30</v>
       </c>
       <c r="B26" s="9">
-        <v>626.5</v>
+        <v>619</v>
       </c>
       <c r="C26" s="12">
-        <v>618.6</v>
+        <v>609.65</v>
       </c>
       <c r="D26" s="15">
-        <v>619.45000000000005</v>
+        <v>611.65</v>
       </c>
       <c r="E26" s="6">
-        <v>620.20000000000005</v>
+        <v>610.95000000000005</v>
       </c>
       <c r="F26" s="18">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="G26" s="6">
-        <v>624.85</v>
+        <v>617.25</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1248,22 +1248,22 @@
         <v>31</v>
       </c>
       <c r="B27" s="9">
-        <v>244.1</v>
+        <v>252.8</v>
       </c>
       <c r="C27" s="12">
-        <v>239.6</v>
+        <v>246.55</v>
       </c>
       <c r="D27" s="15">
-        <v>243.7</v>
+        <v>249.8</v>
       </c>
       <c r="E27" s="6">
-        <v>243.5</v>
+        <v>249.75</v>
       </c>
       <c r="F27" s="18">
-        <v>224</v>
+        <v>286</v>
       </c>
       <c r="G27" s="6">
-        <v>240.75</v>
+        <v>247.35</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1271,22 +1271,22 @@
         <v>32</v>
       </c>
       <c r="B28" s="9">
-        <v>117.75</v>
+        <v>120.1</v>
       </c>
       <c r="C28" s="12">
-        <v>116.5</v>
+        <v>118.05</v>
       </c>
       <c r="D28" s="15">
-        <v>117.55</v>
+        <v>118.3</v>
       </c>
       <c r="E28" s="6">
-        <v>117.55</v>
+        <v>118.25</v>
       </c>
       <c r="F28" s="18">
-        <v>173</v>
+        <v>271</v>
       </c>
       <c r="G28" s="6">
-        <v>116.8</v>
+        <v>119.65</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1294,22 +1294,22 @@
         <v>33</v>
       </c>
       <c r="B29" s="10">
-        <v>8267.9500000000007</v>
+        <v>8324</v>
       </c>
       <c r="C29" s="13">
-        <v>8192.0499999999993</v>
+        <v>8198</v>
       </c>
       <c r="D29" s="16">
-        <v>8198.2999999999993</v>
+        <v>8198</v>
       </c>
       <c r="E29" s="7">
-        <v>8203.5</v>
+        <v>8211.4</v>
       </c>
       <c r="F29" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29" s="7">
-        <v>8230</v>
+        <v>8213.2000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sonia.py date issue fixed(was looking at months as dates)
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>2536.65</v>
+        <v>2465.55</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>2473.55</v>
+        <v>2395.6</v>
       </c>
       <c r="D2" s="14" t="n">
-        <v>2507.6</v>
+        <v>2449.9</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>2506.45</v>
+        <v>2450.05</v>
       </c>
       <c r="F2" s="17" t="n">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>2480.6</v>
+        <v>2401.95</v>
       </c>
     </row>
     <row r="3">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>397.75</v>
+        <v>390.55</v>
       </c>
       <c r="C3" s="12" t="n">
-        <v>388.5</v>
+        <v>383.8</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>389.6</v>
+        <v>385.15</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>389.65</v>
+        <v>384.75</v>
       </c>
       <c r="F3" s="18" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>394.15</v>
+        <v>387.95</v>
       </c>
     </row>
     <row r="4">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
+        <v>1518.7</v>
+      </c>
+      <c r="C4" s="12" t="n">
+        <v>1490.15</v>
+      </c>
+      <c r="D4" s="15" t="n">
         <v>1514</v>
       </c>
-      <c r="C4" s="12" t="n">
-        <v>1497.25</v>
-      </c>
-      <c r="D4" s="15" t="n">
-        <v>1506.95</v>
-      </c>
       <c r="E4" s="6" t="n">
-        <v>1503.45</v>
+        <v>1514.5</v>
       </c>
       <c r="F4" s="18" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>1505.05</v>
+        <v>1493.25</v>
       </c>
     </row>
     <row r="5">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>7310.95</v>
+        <v>7329.4</v>
       </c>
       <c r="C5" s="12" t="n">
-        <v>7236</v>
+        <v>7155</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>7295</v>
+        <v>7300.1</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>7293.35</v>
+        <v>7320.6</v>
       </c>
       <c r="F5" s="18" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>7269</v>
+        <v>7185</v>
       </c>
     </row>
     <row r="6">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>236.7</v>
+        <v>236.25</v>
       </c>
       <c r="C6" s="12" t="n">
-        <v>234.2</v>
+        <v>231.6</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>235.85</v>
+        <v>235.15</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>235.8</v>
+        <v>235.1</v>
       </c>
       <c r="F6" s="18" t="n">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>235.85</v>
+        <v>232.4</v>
       </c>
     </row>
     <row r="7">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>191.6</v>
+        <v>191.8</v>
       </c>
       <c r="C7" s="12" t="n">
-        <v>189.2</v>
+        <v>186.3</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>191.1</v>
+        <v>190.75</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>191.15</v>
+        <v>190.6</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>75</v>
+        <v>158</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>190.75</v>
+        <v>187.6</v>
       </c>
     </row>
     <row r="8">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>230.4</v>
+        <v>237.25</v>
       </c>
       <c r="C8" s="12" t="n">
-        <v>229.25</v>
+        <v>232.1</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>229.85</v>
+        <v>236.9</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>229.95</v>
+        <v>236.9</v>
       </c>
       <c r="F8" s="18" t="n">
-        <v>31</v>
+        <v>148</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>229.55</v>
+        <v>232.4</v>
       </c>
     </row>
     <row r="9">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>497.8</v>
+        <v>509.5</v>
       </c>
       <c r="C9" s="12" t="n">
-        <v>488.5</v>
+        <v>500.3</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>494.5</v>
+        <v>503.9</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>494</v>
+        <v>503.25</v>
       </c>
       <c r="F9" s="18" t="n">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>488.9</v>
+        <v>504.15</v>
       </c>
     </row>
     <row r="10">
@@ -847,22 +847,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>3370</v>
+        <v>3406.45</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>3350</v>
+        <v>3322.1</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>3355</v>
+        <v>3402</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>3355.35</v>
+        <v>3400.4</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>3365</v>
+        <v>3330.05</v>
       </c>
     </row>
     <row r="11">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>146.45</v>
+        <v>144.65</v>
       </c>
       <c r="C11" s="12" t="n">
-        <v>144</v>
+        <v>141.3</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>144.6</v>
+        <v>143.5</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>144.45</v>
+        <v>143.8</v>
       </c>
       <c r="F11" s="18" t="n">
-        <v>172</v>
+        <v>136</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>145</v>
+        <v>143.7</v>
       </c>
     </row>
     <row r="12">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>1163.3</v>
+        <v>1188</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>1148.3</v>
+        <v>1171.1</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>1159</v>
+        <v>1185.1</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>1157.55</v>
+        <v>1185.8</v>
       </c>
       <c r="F12" s="18" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>1150.6</v>
+        <v>1172.1</v>
       </c>
     </row>
     <row r="13">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>1592.65</v>
+        <v>1579</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>1583.45</v>
+        <v>1559.35</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>1591.25</v>
+        <v>1573.75</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>1590.3</v>
+        <v>1574.7</v>
       </c>
       <c r="F13" s="18" t="n">
-        <v>177</v>
+        <v>216</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>1584.3</v>
+        <v>1571.35</v>
       </c>
     </row>
     <row r="14">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>458.5</v>
+        <v>478.5</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>448.55</v>
+        <v>468.75</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>456.9</v>
+        <v>472.7</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>456.05</v>
+        <v>473.25</v>
       </c>
       <c r="F14" s="18" t="n">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>450.75</v>
+        <v>469.75</v>
       </c>
     </row>
     <row r="15">
@@ -972,22 +972,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>976.8</v>
+        <v>973.05</v>
       </c>
       <c r="C15" s="12" t="n">
-        <v>965.65</v>
+        <v>952.8</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>967.7</v>
+        <v>967.6</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>967.75</v>
+        <v>968.7</v>
       </c>
       <c r="F15" s="18" t="n">
-        <v>132</v>
+        <v>162</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>975.3</v>
+        <v>955.6</v>
       </c>
     </row>
     <row r="16">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1409.8</v>
+        <v>1423.6</v>
       </c>
       <c r="C16" s="12" t="n">
-        <v>1392.45</v>
+        <v>1376.3</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>1401</v>
+        <v>1415</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1400.15</v>
+        <v>1416.55</v>
       </c>
       <c r="F16" s="18" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1409.55</v>
+        <v>1383.35</v>
       </c>
     </row>
     <row r="17">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1424</v>
+        <v>1446</v>
       </c>
       <c r="C17" s="12" t="n">
-        <v>1415.3</v>
+        <v>1428.2</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>1418</v>
+        <v>1442</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1417.65</v>
+        <v>1443.85</v>
       </c>
       <c r="F17" s="18" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1421.8</v>
+        <v>1429.55</v>
       </c>
     </row>
     <row r="18">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>679.7</v>
+        <v>713.7</v>
       </c>
       <c r="C18" s="12" t="n">
-        <v>659</v>
+        <v>691.05</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>675.5</v>
+        <v>701</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>676.3</v>
+        <v>701.1</v>
       </c>
       <c r="F18" s="18" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>662.4</v>
+        <v>692.95</v>
       </c>
     </row>
     <row r="19">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>426.5</v>
+        <v>435.85</v>
       </c>
       <c r="C19" s="12" t="n">
-        <v>419</v>
+        <v>425.2</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>423.1</v>
+        <v>434.1</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>423.3</v>
+        <v>433.2</v>
       </c>
       <c r="F19" s="18" t="n">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>420.25</v>
+        <v>425.7</v>
       </c>
     </row>
     <row r="20">
@@ -1097,22 +1097,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>1564.35</v>
+        <v>1604.5</v>
       </c>
       <c r="C20" s="12" t="n">
-        <v>1540</v>
+        <v>1582.4</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>1555.05</v>
+        <v>1589.95</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>1560.85</v>
+        <v>1591.95</v>
       </c>
       <c r="F20" s="18" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>1549.25</v>
+        <v>1599.05</v>
       </c>
     </row>
     <row r="21">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>295.35</v>
+        <v>300.2</v>
       </c>
       <c r="C21" s="12" t="n">
-        <v>291.4</v>
+        <v>293.85</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>293.25</v>
+        <v>298.6</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>293.15</v>
+        <v>299.15</v>
       </c>
       <c r="F21" s="18" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>294.7</v>
+        <v>296.6</v>
       </c>
     </row>
     <row r="22">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>2437.6</v>
+        <v>2425.65</v>
       </c>
       <c r="C22" s="12" t="n">
-        <v>2408.15</v>
+        <v>2402.1</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>2422</v>
+        <v>2411.4</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>2420.35</v>
+        <v>2412.65</v>
       </c>
       <c r="F22" s="18" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>2428</v>
+        <v>2411.85</v>
       </c>
     </row>
     <row r="23">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>576.3</v>
+        <v>571.2</v>
       </c>
       <c r="C23" s="12" t="n">
-        <v>571.85</v>
+        <v>562.3</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>575.25</v>
+        <v>569.5</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>574.85</v>
+        <v>569.55</v>
       </c>
       <c r="F23" s="18" t="n">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>572.8</v>
+        <v>564.5</v>
       </c>
     </row>
     <row r="24">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>605</v>
+        <v>623.75</v>
       </c>
       <c r="C24" s="12" t="n">
-        <v>595.3</v>
+        <v>615.35</v>
       </c>
       <c r="D24" s="15" t="n">
-        <v>604.1</v>
+        <v>619.55</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>604.2</v>
+        <v>620.8</v>
       </c>
       <c r="F24" s="18" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>601.1</v>
+        <v>617.8</v>
       </c>
     </row>
     <row r="25">
@@ -1222,22 +1222,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C25" s="12" t="n">
-        <v>1061.45</v>
+        <v>1064</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>1069.65</v>
+        <v>1071</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>1066.9</v>
+        <v>1071.15</v>
       </c>
       <c r="F25" s="18" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>1063</v>
+        <v>1068.25</v>
       </c>
     </row>
     <row r="26">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>610.5</v>
+        <v>614.9</v>
       </c>
       <c r="C26" s="12" t="n">
-        <v>605.1</v>
+        <v>603.7</v>
       </c>
       <c r="D26" s="15" t="n">
-        <v>607.65</v>
+        <v>610.4</v>
       </c>
       <c r="E26" s="6" t="n">
-        <v>607.15</v>
+        <v>611.2</v>
       </c>
       <c r="F26" s="18" t="n">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="G26" s="6" t="n">
-        <v>606.65</v>
+        <v>604.05</v>
       </c>
     </row>
     <row r="27">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>248.5</v>
+        <v>255.95</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>245.9</v>
+        <v>247.6</v>
       </c>
       <c r="D27" s="15" t="n">
-        <v>246.8</v>
+        <v>255.5</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>246.9</v>
+        <v>255.35</v>
       </c>
       <c r="F27" s="18" t="n">
-        <v>72</v>
+        <v>280</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>247.2</v>
+        <v>247.75</v>
       </c>
     </row>
     <row r="28">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>120.15</v>
+        <v>128.7</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>117.75</v>
+        <v>125.4</v>
       </c>
       <c r="D28" s="15" t="n">
-        <v>119.8</v>
+        <v>126.8</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>119.55</v>
+        <v>127.05</v>
       </c>
       <c r="F28" s="18" t="n">
-        <v>360</v>
+        <v>764</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>118.1</v>
+        <v>125.7</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" thickBot="1">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B29" s="10" t="n">
-        <v>8218</v>
+        <v>8339.799999999999</v>
       </c>
       <c r="C29" s="13" t="n">
-        <v>8152.7</v>
+        <v>8249</v>
       </c>
       <c r="D29" s="16" t="n">
-        <v>8200</v>
+        <v>8269.9</v>
       </c>
       <c r="E29" s="7" t="n">
-        <v>8199.700000000001</v>
+        <v>8262.4</v>
       </c>
       <c r="F29" s="19" t="n">
         <v>2</v>
       </c>
       <c r="G29" s="7" t="n">
-        <v>8163.65</v>
+        <v>8312.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added leetcode sheets to practice leetcode
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>2465.55</v>
+        <v>2504</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>2395.6</v>
+        <v>2471</v>
       </c>
       <c r="D2" s="14" t="n">
-        <v>2449.9</v>
+        <v>2489.45</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>2450.05</v>
+        <v>2496.5</v>
       </c>
       <c r="F2" s="17" t="n">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>2401.95</v>
+        <v>2478.55</v>
       </c>
     </row>
     <row r="3">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>390.55</v>
+        <v>384.85</v>
       </c>
       <c r="C3" s="12" t="n">
-        <v>383.8</v>
+        <v>376</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>385.15</v>
+        <v>382</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>384.75</v>
+        <v>382.25</v>
       </c>
       <c r="F3" s="18" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>387.95</v>
+        <v>376.45</v>
       </c>
     </row>
     <row r="4">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>1518.7</v>
+        <v>1522.45</v>
       </c>
       <c r="C4" s="12" t="n">
-        <v>1490.15</v>
+        <v>1504.2</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>1514</v>
+        <v>1519</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>1514.5</v>
+        <v>1518.2</v>
       </c>
       <c r="F4" s="18" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>1493.25</v>
+        <v>1510.45</v>
       </c>
     </row>
     <row r="5">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>7329.4</v>
+        <v>7397</v>
       </c>
       <c r="C5" s="12" t="n">
-        <v>7155</v>
+        <v>7296</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>7300.1</v>
+        <v>7391</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>7320.6</v>
+        <v>7387.8</v>
       </c>
       <c r="F5" s="18" t="n">
         <v>6</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>7185</v>
+        <v>7303.7</v>
       </c>
     </row>
     <row r="6">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>236.25</v>
+        <v>236.15</v>
       </c>
       <c r="C6" s="12" t="n">
-        <v>231.6</v>
+        <v>232.3</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>235.15</v>
+        <v>233.9</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>235.1</v>
+        <v>234</v>
       </c>
       <c r="F6" s="18" t="n">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>232.4</v>
+        <v>235.05</v>
       </c>
     </row>
     <row r="7">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>191.8</v>
+        <v>197.55</v>
       </c>
       <c r="C7" s="12" t="n">
-        <v>186.3</v>
+        <v>194</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>190.75</v>
+        <v>194.55</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>190.6</v>
+        <v>195</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>187.6</v>
+        <v>195.55</v>
       </c>
     </row>
     <row r="8">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>237.25</v>
+        <v>257.8</v>
       </c>
       <c r="C8" s="12" t="n">
-        <v>232.1</v>
+        <v>252.55</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>236.9</v>
+        <v>255.25</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>236.9</v>
+        <v>255.8</v>
       </c>
       <c r="F8" s="18" t="n">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>232.4</v>
+        <v>257.25</v>
       </c>
     </row>
     <row r="9">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>509.5</v>
+        <v>522.5</v>
       </c>
       <c r="C9" s="12" t="n">
-        <v>500.3</v>
+        <v>513.8</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>503.9</v>
+        <v>519</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>503.25</v>
+        <v>519</v>
       </c>
       <c r="F9" s="18" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>504.15</v>
+        <v>519.65</v>
       </c>
     </row>
     <row r="10">
@@ -847,22 +847,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>3406.45</v>
+        <v>3417.1</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>3322.1</v>
+        <v>3375</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>3402</v>
+        <v>3390</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>3400.4</v>
+        <v>3391.3</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>3330.05</v>
+        <v>3408.4</v>
       </c>
     </row>
     <row r="11">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>144.65</v>
+        <v>145.5</v>
       </c>
       <c r="C11" s="12" t="n">
-        <v>141.3</v>
+        <v>142.85</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>143.5</v>
+        <v>143.9</v>
       </c>
       <c r="E11" s="6" t="n">
         <v>143.8</v>
       </c>
       <c r="F11" s="18" t="n">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>143.7</v>
+        <v>144.7</v>
       </c>
     </row>
     <row r="12">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>1188</v>
+        <v>1241.55</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>1171.1</v>
+        <v>1222.7</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>1185.1</v>
+        <v>1236</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>1185.8</v>
+        <v>1235.85</v>
       </c>
       <c r="F12" s="18" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>1172.1</v>
+        <v>1239.1</v>
       </c>
     </row>
     <row r="13">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>1579</v>
+        <v>1600</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>1559.35</v>
+        <v>1580.35</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>1573.75</v>
+        <v>1599</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>1574.7</v>
+        <v>1595.5</v>
       </c>
       <c r="F13" s="18" t="n">
-        <v>216</v>
+        <v>281</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>1571.35</v>
+        <v>1582.25</v>
       </c>
     </row>
     <row r="14">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>478.5</v>
+        <v>480.55</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>468.75</v>
+        <v>474.25</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>472.7</v>
+        <v>478.1</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>473.25</v>
+        <v>478.15</v>
       </c>
       <c r="F14" s="18" t="n">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>469.75</v>
+        <v>479.55</v>
       </c>
     </row>
     <row r="15">
@@ -972,22 +972,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>973.05</v>
+        <v>966.35</v>
       </c>
       <c r="C15" s="12" t="n">
-        <v>952.8</v>
+        <v>950.8</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>967.6</v>
+        <v>960.05</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>968.7</v>
+        <v>957.5</v>
       </c>
       <c r="F15" s="18" t="n">
-        <v>162</v>
+        <v>308</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>955.6</v>
+        <v>964.45</v>
       </c>
     </row>
     <row r="16">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1423.6</v>
+        <v>1416.9</v>
       </c>
       <c r="C16" s="12" t="n">
-        <v>1376.3</v>
+        <v>1396.45</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>1415</v>
+        <v>1405.25</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1416.55</v>
+        <v>1408.65</v>
       </c>
       <c r="F16" s="18" t="n">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1383.35</v>
+        <v>1409.9</v>
       </c>
     </row>
     <row r="17">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1446</v>
+        <v>1480.25</v>
       </c>
       <c r="C17" s="12" t="n">
-        <v>1428.2</v>
+        <v>1463.3</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>1442</v>
+        <v>1475.8</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1443.85</v>
+        <v>1477.45</v>
       </c>
       <c r="F17" s="18" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1429.55</v>
+        <v>1475.05</v>
       </c>
     </row>
     <row r="18">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>713.7</v>
+        <v>704.45</v>
       </c>
       <c r="C18" s="12" t="n">
-        <v>691.05</v>
+        <v>697</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>701</v>
+        <v>701.25</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>701.1</v>
+        <v>702.45</v>
       </c>
       <c r="F18" s="18" t="n">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>692.95</v>
+        <v>701.55</v>
       </c>
     </row>
     <row r="19">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>435.85</v>
+        <v>454</v>
       </c>
       <c r="C19" s="12" t="n">
-        <v>425.2</v>
+        <v>445</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>434.1</v>
+        <v>449.6</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>433.2</v>
+        <v>449.25</v>
       </c>
       <c r="F19" s="18" t="n">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>425.7</v>
+        <v>452.8</v>
       </c>
     </row>
     <row r="20">
@@ -1097,22 +1097,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>1604.5</v>
+        <v>1580.9</v>
       </c>
       <c r="C20" s="12" t="n">
-        <v>1582.4</v>
+        <v>1558.7</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>1589.95</v>
+        <v>1572.2</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>1591.95</v>
+        <v>1577</v>
       </c>
       <c r="F20" s="18" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>1599.05</v>
+        <v>1567.9</v>
       </c>
     </row>
     <row r="21">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>300.2</v>
+        <v>294.8</v>
       </c>
       <c r="C21" s="12" t="n">
-        <v>293.85</v>
+        <v>289.05</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>298.6</v>
+        <v>294</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>299.15</v>
+        <v>294.35</v>
       </c>
       <c r="F21" s="18" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>296.6</v>
+        <v>293.6</v>
       </c>
     </row>
     <row r="22">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>2425.65</v>
+        <v>2436.15</v>
       </c>
       <c r="C22" s="12" t="n">
-        <v>2402.1</v>
+        <v>2417.25</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>2411.4</v>
+        <v>2426.35</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>2412.65</v>
+        <v>2428.7</v>
       </c>
       <c r="F22" s="18" t="n">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>2411.85</v>
+        <v>2428.45</v>
       </c>
     </row>
     <row r="23">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>571.2</v>
+        <v>573.85</v>
       </c>
       <c r="C23" s="12" t="n">
-        <v>562.3</v>
+        <v>568</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>569.5</v>
+        <v>570.95</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>569.55</v>
+        <v>570.5</v>
       </c>
       <c r="F23" s="18" t="n">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>564.5</v>
+        <v>572.3</v>
       </c>
     </row>
     <row r="24">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>623.75</v>
+        <v>619.55</v>
       </c>
       <c r="C24" s="12" t="n">
+        <v>607</v>
+      </c>
+      <c r="D24" s="15" t="n">
+        <v>614</v>
+      </c>
+      <c r="E24" s="6" t="n">
         <v>615.35</v>
-      </c>
-      <c r="D24" s="15" t="n">
-        <v>619.55</v>
-      </c>
-      <c r="E24" s="6" t="n">
-        <v>620.8</v>
       </c>
       <c r="F24" s="18" t="n">
         <v>9</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>617.8</v>
+        <v>614.15</v>
       </c>
     </row>
     <row r="25">
@@ -1222,22 +1222,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>1076</v>
+        <v>1099.25</v>
       </c>
       <c r="C25" s="12" t="n">
-        <v>1064</v>
+        <v>1078.2</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>1071</v>
+        <v>1090</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>1071.15</v>
+        <v>1090.1</v>
       </c>
       <c r="F25" s="18" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>1068.25</v>
+        <v>1097.45</v>
       </c>
     </row>
     <row r="26">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>614.9</v>
+        <v>611.45</v>
       </c>
       <c r="C26" s="12" t="n">
-        <v>603.7</v>
+        <v>605.6</v>
       </c>
       <c r="D26" s="15" t="n">
-        <v>610.4</v>
+        <v>610.6</v>
       </c>
       <c r="E26" s="6" t="n">
-        <v>611.2</v>
+        <v>610.25</v>
       </c>
       <c r="F26" s="18" t="n">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="G26" s="6" t="n">
-        <v>604.05</v>
+        <v>608.9</v>
       </c>
     </row>
     <row r="27">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>255.95</v>
+        <v>259.75</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>247.6</v>
+        <v>254.65</v>
       </c>
       <c r="D27" s="15" t="n">
-        <v>255.5</v>
+        <v>257.1</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>255.35</v>
+        <v>257.5</v>
       </c>
       <c r="F27" s="18" t="n">
-        <v>280</v>
+        <v>92</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>247.75</v>
+        <v>258.85</v>
       </c>
     </row>
     <row r="28">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>128.7</v>
+        <v>131.05</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>125.4</v>
+        <v>128.2</v>
       </c>
       <c r="D28" s="15" t="n">
-        <v>126.8</v>
+        <v>129.45</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>127.05</v>
+        <v>129.6</v>
       </c>
       <c r="F28" s="18" t="n">
-        <v>764</v>
+        <v>360</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>125.7</v>
+        <v>130.8</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" thickBot="1">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B29" s="10" t="n">
-        <v>8339.799999999999</v>
+        <v>8556.799999999999</v>
       </c>
       <c r="C29" s="13" t="n">
-        <v>8249</v>
+        <v>8444.1</v>
       </c>
       <c r="D29" s="16" t="n">
-        <v>8269.9</v>
+        <v>8550</v>
       </c>
       <c r="E29" s="7" t="n">
-        <v>8262.4</v>
+        <v>8537.4</v>
       </c>
       <c r="F29" s="19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G29" s="7" t="n">
-        <v>8312.1</v>
+        <v>8508.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added xls to xlsx in python itself and a running backup of xls hourlys every day
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>2504</v>
+        <v>2520</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>2471</v>
+        <v>2485</v>
       </c>
       <c r="D2" s="14" t="n">
-        <v>2489.45</v>
+        <v>2506</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>2496.5</v>
+        <v>2509.5</v>
       </c>
       <c r="F2" s="17" t="n">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>2478.55</v>
+        <v>2495.4</v>
       </c>
     </row>
     <row r="3">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>384.85</v>
+        <v>387.6</v>
       </c>
       <c r="C3" s="12" t="n">
-        <v>376</v>
+        <v>382.7</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>382</v>
+        <v>384.15</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>382.25</v>
+        <v>384.3</v>
       </c>
       <c r="F3" s="18" t="n">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>376.45</v>
+        <v>383.2</v>
       </c>
     </row>
     <row r="4">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>1522.45</v>
+        <v>1522.95</v>
       </c>
       <c r="C4" s="12" t="n">
-        <v>1504.2</v>
+        <v>1510.1</v>
       </c>
       <c r="D4" s="15" t="n">
         <v>1519</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>1518.2</v>
+        <v>1519.55</v>
       </c>
       <c r="F4" s="18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>1510.45</v>
+        <v>1515.45</v>
       </c>
     </row>
     <row r="5">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>7397</v>
+        <v>7375</v>
       </c>
       <c r="C5" s="12" t="n">
-        <v>7296</v>
+        <v>7303.7</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>7391</v>
+        <v>7363</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>7387.8</v>
+        <v>7363.2</v>
       </c>
       <c r="F5" s="18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>7303.7</v>
+        <v>7332.9</v>
       </c>
     </row>
     <row r="6">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>236.15</v>
+        <v>239.15</v>
       </c>
       <c r="C6" s="12" t="n">
-        <v>232.3</v>
+        <v>232.4</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>233.9</v>
+        <v>238.5</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>234</v>
+        <v>238.5</v>
       </c>
       <c r="F6" s="18" t="n">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>235.05</v>
+        <v>233.85</v>
       </c>
     </row>
     <row r="7">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>197.55</v>
+        <v>196.75</v>
       </c>
       <c r="C7" s="12" t="n">
-        <v>194</v>
+        <v>194.55</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>194.55</v>
+        <v>196.2</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>195</v>
+        <v>196.25</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>156</v>
+        <v>105</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>195.55</v>
+        <v>194.6</v>
       </c>
     </row>
     <row r="8">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>257.8</v>
+        <v>274.75</v>
       </c>
       <c r="C8" s="12" t="n">
-        <v>252.55</v>
+        <v>257.1</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>255.25</v>
+        <v>273.5</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>255.8</v>
+        <v>274</v>
       </c>
       <c r="F8" s="18" t="n">
-        <v>133</v>
+        <v>722</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>257.25</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>522.5</v>
+        <v>532.5</v>
       </c>
       <c r="C9" s="12" t="n">
-        <v>513.8</v>
+        <v>514.55</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>519</v>
+        <v>531.5</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>519</v>
+        <v>530.75</v>
       </c>
       <c r="F9" s="18" t="n">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>519.65</v>
+        <v>518.55</v>
       </c>
     </row>
     <row r="10">
@@ -847,22 +847,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>3417.1</v>
+        <v>3411.95</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>3375</v>
+        <v>3375.05</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>3390</v>
+        <v>3397.4</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>3391.3</v>
+        <v>3402.45</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>3408.4</v>
+        <v>3382.4</v>
       </c>
     </row>
     <row r="11">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>145.5</v>
+        <v>147.15</v>
       </c>
       <c r="C11" s="12" t="n">
-        <v>142.85</v>
+        <v>144.15</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>143.9</v>
+        <v>145.25</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>143.8</v>
+        <v>145</v>
       </c>
       <c r="F11" s="18" t="n">
-        <v>173</v>
+        <v>131</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>144.7</v>
+        <v>144.15</v>
       </c>
     </row>
     <row r="12">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>1241.55</v>
+        <v>1257</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>1222.7</v>
+        <v>1230.45</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>1236</v>
+        <v>1255</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>1235.85</v>
+        <v>1254</v>
       </c>
       <c r="F12" s="18" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>1239.1</v>
+        <v>1233.3</v>
       </c>
     </row>
     <row r="13">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>1600</v>
+        <v>1614</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>1580.35</v>
+        <v>1587.15</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>1599</v>
+        <v>1611</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>1595.5</v>
+        <v>1610.85</v>
       </c>
       <c r="F13" s="18" t="n">
-        <v>281</v>
+        <v>171</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>1582.25</v>
+        <v>1588.5</v>
       </c>
     </row>
     <row r="14">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>480.55</v>
+        <v>479.5</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>474.25</v>
+        <v>473.55</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>478.1</v>
+        <v>475.1</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>478.15</v>
+        <v>475.1</v>
       </c>
       <c r="F14" s="18" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>479.55</v>
+        <v>476.15</v>
       </c>
     </row>
     <row r="15">
@@ -972,22 +972,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>966.35</v>
+        <v>969.5</v>
       </c>
       <c r="C15" s="12" t="n">
-        <v>950.8</v>
+        <v>955.05</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>960.05</v>
+        <v>962.95</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>957.5</v>
+        <v>965.65</v>
       </c>
       <c r="F15" s="18" t="n">
-        <v>308</v>
+        <v>134</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>964.45</v>
+        <v>956.7</v>
       </c>
     </row>
     <row r="16">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1416.9</v>
+        <v>1443.2</v>
       </c>
       <c r="C16" s="12" t="n">
-        <v>1396.45</v>
+        <v>1401.6</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>1405.25</v>
+        <v>1438</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1408.65</v>
+        <v>1439.6</v>
       </c>
       <c r="F16" s="18" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1409.9</v>
+        <v>1403.25</v>
       </c>
     </row>
     <row r="17">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1480.25</v>
+        <v>1472</v>
       </c>
       <c r="C17" s="12" t="n">
-        <v>1463.3</v>
+        <v>1462.05</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>1475.8</v>
+        <v>1467.3</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1477.45</v>
+        <v>1466.2</v>
       </c>
       <c r="F17" s="18" t="n">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1475.05</v>
+        <v>1469.9</v>
       </c>
     </row>
     <row r="18">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>704.45</v>
+        <v>707.75</v>
       </c>
       <c r="C18" s="12" t="n">
-        <v>697</v>
+        <v>700.1</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>701.25</v>
+        <v>701.8</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>702.45</v>
+        <v>703.5</v>
       </c>
       <c r="F18" s="18" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>701.55</v>
+        <v>701.05</v>
       </c>
     </row>
     <row r="19">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>454</v>
+        <v>454.95</v>
       </c>
       <c r="C19" s="12" t="n">
-        <v>445</v>
+        <v>444.95</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>449.6</v>
+        <v>451</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>449.25</v>
+        <v>451</v>
       </c>
       <c r="F19" s="18" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>452.8</v>
+        <v>449.85</v>
       </c>
     </row>
     <row r="20">
@@ -1097,22 +1097,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>1580.9</v>
+        <v>1574.45</v>
       </c>
       <c r="C20" s="12" t="n">
-        <v>1558.7</v>
+        <v>1560.25</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>1572.2</v>
+        <v>1564.9</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>1577</v>
+        <v>1565.75</v>
       </c>
       <c r="F20" s="18" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>1567.9</v>
+        <v>1571.8</v>
       </c>
     </row>
     <row r="21">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>294.8</v>
+        <v>301</v>
       </c>
       <c r="C21" s="12" t="n">
-        <v>289.05</v>
+        <v>293.3</v>
       </c>
       <c r="D21" s="15" t="n">
+        <v>300.9</v>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v>299.9</v>
+      </c>
+      <c r="F21" s="18" t="n">
+        <v>33</v>
+      </c>
+      <c r="G21" s="6" t="n">
         <v>294</v>
-      </c>
-      <c r="E21" s="6" t="n">
-        <v>294.35</v>
-      </c>
-      <c r="F21" s="18" t="n">
-        <v>26</v>
-      </c>
-      <c r="G21" s="6" t="n">
-        <v>293.6</v>
       </c>
     </row>
     <row r="22">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>2436.15</v>
+        <v>2438.25</v>
       </c>
       <c r="C22" s="12" t="n">
-        <v>2417.25</v>
+        <v>2411</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>2426.35</v>
+        <v>2431</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>2428.7</v>
+        <v>2432</v>
       </c>
       <c r="F22" s="18" t="n">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>2428.45</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="23">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>573.85</v>
+        <v>581</v>
       </c>
       <c r="C23" s="12" t="n">
-        <v>568</v>
+        <v>571.9</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>570.95</v>
+        <v>580.6</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>570.5</v>
+        <v>579.05</v>
       </c>
       <c r="F23" s="18" t="n">
-        <v>206</v>
+        <v>123</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>572.3</v>
+        <v>572.15</v>
       </c>
     </row>
     <row r="24">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>619.55</v>
+        <v>623.85</v>
       </c>
       <c r="C24" s="12" t="n">
-        <v>607</v>
+        <v>612.6</v>
       </c>
       <c r="D24" s="15" t="n">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>615.35</v>
+        <v>617.35</v>
       </c>
       <c r="F24" s="18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>614.15</v>
+        <v>620.65</v>
       </c>
     </row>
     <row r="25">
@@ -1222,22 +1222,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>1099.25</v>
+        <v>1088.25</v>
       </c>
       <c r="C25" s="12" t="n">
         <v>1078.2</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>1090</v>
+        <v>1085.15</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>1090.1</v>
+        <v>1086.15</v>
       </c>
       <c r="F25" s="18" t="n">
         <v>6</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>1097.45</v>
+        <v>1082.35</v>
       </c>
     </row>
     <row r="26">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>611.45</v>
+        <v>616.5</v>
       </c>
       <c r="C26" s="12" t="n">
-        <v>605.6</v>
+        <v>609.05</v>
       </c>
       <c r="D26" s="15" t="n">
-        <v>610.6</v>
+        <v>614.25</v>
       </c>
       <c r="E26" s="6" t="n">
-        <v>610.25</v>
+        <v>614.9</v>
       </c>
       <c r="F26" s="18" t="n">
         <v>65</v>
       </c>
       <c r="G26" s="6" t="n">
-        <v>608.9</v>
+        <v>609.2</v>
       </c>
     </row>
     <row r="27">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>259.75</v>
+        <v>266.35</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>254.65</v>
+        <v>256.3</v>
       </c>
       <c r="D27" s="15" t="n">
-        <v>257.1</v>
+        <v>263.65</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>257.5</v>
+        <v>263.7</v>
       </c>
       <c r="F27" s="18" t="n">
-        <v>92</v>
+        <v>177</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>258.85</v>
+        <v>257.2</v>
       </c>
     </row>
     <row r="28">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>131.05</v>
+        <v>130.8</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>128.2</v>
+        <v>128.75</v>
       </c>
       <c r="D28" s="15" t="n">
-        <v>129.45</v>
+        <v>130.1</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>129.6</v>
+        <v>130.15</v>
       </c>
       <c r="F28" s="18" t="n">
-        <v>360</v>
+        <v>302</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>130.8</v>
+        <v>128.8</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" thickBot="1">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B29" s="10" t="n">
-        <v>8556.799999999999</v>
+        <v>8515.75</v>
       </c>
       <c r="C29" s="13" t="n">
-        <v>8444.1</v>
+        <v>8430</v>
       </c>
       <c r="D29" s="16" t="n">
-        <v>8550</v>
+        <v>8482.5</v>
       </c>
       <c r="E29" s="7" t="n">
-        <v>8537.4</v>
+        <v>8495.15</v>
       </c>
       <c r="F29" s="19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29" s="7" t="n">
-        <v>8508.85</v>
+        <v>8475.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added modular amount option to calc
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -598,7 +598,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>2404.65</v>
+        <v>2260</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>2301.8</v>
+        <v>2226.65</v>
       </c>
       <c r="D2" s="14" t="n">
-        <v>2304.95</v>
+        <v>2235.45</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>2308.65</v>
+        <v>2233.35</v>
       </c>
       <c r="F2" s="17" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>2397.1</v>
+        <v>2252.8</v>
       </c>
     </row>
     <row r="3">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>385.4</v>
+        <v>389.55</v>
       </c>
       <c r="C3" s="12" t="n">
-        <v>371.7</v>
+        <v>382</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>375</v>
+        <v>384.95</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>375</v>
+        <v>384.1</v>
       </c>
       <c r="F3" s="18" t="n">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>384.45</v>
+        <v>389.2</v>
       </c>
     </row>
     <row r="4">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>1651.7</v>
+        <v>1595</v>
       </c>
       <c r="C4" s="12" t="n">
-        <v>1605.5</v>
+        <v>1550</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>1607</v>
+        <v>1569.9</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>1613.15</v>
+        <v>1569.8</v>
       </c>
       <c r="F4" s="18" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>1648.85</v>
+        <v>1588.5</v>
       </c>
     </row>
     <row r="5">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>7884.9</v>
+        <v>7634.5</v>
       </c>
       <c r="C5" s="12" t="n">
-        <v>7769.9</v>
+        <v>7446</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>7775</v>
+        <v>7499</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>7798.9</v>
+        <v>7495.6</v>
       </c>
       <c r="F5" s="18" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>7860.05</v>
+        <v>7611.75</v>
       </c>
     </row>
     <row r="6">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>228.45</v>
+        <v>218.95</v>
       </c>
       <c r="C6" s="12" t="n">
-        <v>220.4</v>
+        <v>215.65</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>221.5</v>
+        <v>216.4</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>221.3</v>
+        <v>216.1</v>
       </c>
       <c r="F6" s="18" t="n">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>227.65</v>
+        <v>217.9</v>
       </c>
     </row>
     <row r="7">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>202.9</v>
+        <v>194.6</v>
       </c>
       <c r="C7" s="12" t="n">
-        <v>194</v>
+        <v>190.65</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>194.75</v>
+        <v>191.8</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>195.2</v>
+        <v>191.25</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>157</v>
+        <v>513</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>202.8</v>
+        <v>194.1</v>
       </c>
     </row>
     <row r="8">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>312.45</v>
+        <v>318.8</v>
       </c>
       <c r="C8" s="12" t="n">
-        <v>305</v>
+        <v>313.65</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>305.5</v>
+        <v>314.75</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>306.1</v>
+        <v>314.25</v>
       </c>
       <c r="F8" s="18" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>311</v>
+        <v>315.7</v>
       </c>
     </row>
     <row r="9">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>555.65</v>
+        <v>594.5</v>
       </c>
       <c r="C9" s="12" t="n">
-        <v>531.25</v>
+        <v>586.5</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>532</v>
+        <v>591.8</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>532.95</v>
+        <v>592.45</v>
       </c>
       <c r="F9" s="18" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>552.65</v>
+        <v>588</v>
       </c>
     </row>
     <row r="10">
@@ -847,22 +847,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>3492.9</v>
+        <v>3538.95</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>3425.85</v>
+        <v>3485</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>3438.9</v>
+        <v>3515</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>3446.35</v>
+        <v>3509.05</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>3490.2</v>
+        <v>3505.8</v>
       </c>
     </row>
     <row r="11">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>146.1</v>
+        <v>148.2</v>
       </c>
       <c r="C11" s="12" t="n">
-        <v>142.5</v>
+        <v>143.85</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>142.85</v>
+        <v>147.8</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>143.4</v>
+        <v>147.3</v>
       </c>
       <c r="F11" s="18" t="n">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>145.85</v>
+        <v>144.1</v>
       </c>
     </row>
     <row r="12">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>1260.5</v>
+        <v>1277.7</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>1232.3</v>
+        <v>1267.1</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>1234.95</v>
+        <v>1275</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>1236.65</v>
+        <v>1273.95</v>
       </c>
       <c r="F12" s="18" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>1257.5</v>
+        <v>1274.9</v>
       </c>
     </row>
     <row r="13">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>1527.75</v>
+        <v>1490.4</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>1500.1</v>
+        <v>1477.2</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>1507</v>
+        <v>1490</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>1506.05</v>
+        <v>1487.25</v>
       </c>
       <c r="F13" s="18" t="n">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>1526.85</v>
+        <v>1485.4</v>
       </c>
     </row>
     <row r="14">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>473.95</v>
+        <v>491.5</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>455</v>
+        <v>482.35</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>457.25</v>
+        <v>483.95</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>456.7</v>
+        <v>484.55</v>
       </c>
       <c r="F14" s="18" t="n">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>472.5</v>
+        <v>483.4</v>
       </c>
     </row>
     <row r="15">
@@ -972,22 +972,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>943.7</v>
+        <v>950.45</v>
       </c>
       <c r="C15" s="12" t="n">
-        <v>925.4</v>
+        <v>930.45</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>931.1</v>
+        <v>948.35</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>929.95</v>
+        <v>948.1</v>
       </c>
       <c r="F15" s="18" t="n">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>940.5</v>
+        <v>939.75</v>
       </c>
     </row>
     <row r="16">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1468.95</v>
+        <v>1490.45</v>
       </c>
       <c r="C16" s="12" t="n">
-        <v>1430.05</v>
+        <v>1466</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>1445</v>
+        <v>1486.45</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1435</v>
+        <v>1486.4</v>
       </c>
       <c r="F16" s="18" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1467.35</v>
+        <v>1474.45</v>
       </c>
     </row>
     <row r="17">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1429.95</v>
+        <v>1405.9</v>
       </c>
       <c r="C17" s="12" t="n">
-        <v>1405.25</v>
+        <v>1395.9</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>1409</v>
+        <v>1404.5</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1408.65</v>
+        <v>1404.3</v>
       </c>
       <c r="F17" s="18" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1428.05</v>
+        <v>1397.45</v>
       </c>
     </row>
     <row r="18">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>664</v>
+        <v>633.5</v>
       </c>
       <c r="C18" s="12" t="n">
-        <v>637.05</v>
+        <v>620.55</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>638.55</v>
+        <v>630.15</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>640.15</v>
+        <v>630.35</v>
       </c>
       <c r="F18" s="18" t="n">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>662.7</v>
+        <v>621.55</v>
       </c>
     </row>
     <row r="19">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>460</v>
+        <v>465.15</v>
       </c>
       <c r="C19" s="12" t="n">
-        <v>448.75</v>
+        <v>457.35</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>450</v>
+        <v>460.7</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>451.85</v>
+        <v>461</v>
       </c>
       <c r="F19" s="18" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>459.7</v>
+        <v>464.6</v>
       </c>
     </row>
     <row r="20">
@@ -1097,22 +1097,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>1574.9</v>
+        <v>1497</v>
       </c>
       <c r="C20" s="12" t="n">
-        <v>1558.45</v>
+        <v>1475</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>1561</v>
+        <v>1479.6</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>1565.15</v>
+        <v>1479.75</v>
       </c>
       <c r="F20" s="18" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>1569.6</v>
+        <v>1486.8</v>
       </c>
     </row>
     <row r="21">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>279.7</v>
+        <v>264.9</v>
       </c>
       <c r="C21" s="12" t="n">
-        <v>271.3</v>
+        <v>258.9</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>272.05</v>
+        <v>264</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>272.8</v>
+        <v>263.95</v>
       </c>
       <c r="F21" s="18" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>277.55</v>
+        <v>261.65</v>
       </c>
     </row>
     <row r="22">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>2306.25</v>
+        <v>2339.1</v>
       </c>
       <c r="C22" s="12" t="n">
-        <v>2255.25</v>
+        <v>2319.55</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>2262.9</v>
+        <v>2323.1</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>2263.2</v>
+        <v>2323.8</v>
       </c>
       <c r="F22" s="18" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>2295</v>
+        <v>2338.7</v>
       </c>
     </row>
     <row r="23">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>564.2</v>
+        <v>581.2</v>
       </c>
       <c r="C23" s="12" t="n">
-        <v>551</v>
+        <v>574.3</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>552.4</v>
+        <v>580.35</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>552.95</v>
+        <v>579.75</v>
       </c>
       <c r="F23" s="18" t="n">
-        <v>118</v>
+        <v>179</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>563.45</v>
+        <v>574.7</v>
       </c>
     </row>
     <row r="24">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>648</v>
+        <v>654.85</v>
       </c>
       <c r="C24" s="12" t="n">
-        <v>625</v>
+        <v>647.05</v>
       </c>
       <c r="D24" s="15" t="n">
-        <v>627.3</v>
+        <v>652.35</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>631.6</v>
+        <v>652.3</v>
       </c>
       <c r="F24" s="18" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>647.05</v>
+        <v>649.15</v>
       </c>
     </row>
     <row r="25">
@@ -1222,22 +1222,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>1013.1</v>
+        <v>969.7</v>
       </c>
       <c r="C25" s="12" t="n">
-        <v>975.05</v>
+        <v>961</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>980</v>
+        <v>964</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>978.5</v>
+        <v>963.7</v>
       </c>
       <c r="F25" s="18" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>1011.45</v>
+        <v>967.55</v>
       </c>
     </row>
     <row r="26">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>665.95</v>
+        <v>649.9</v>
       </c>
       <c r="C26" s="12" t="n">
+        <v>643.3</v>
+      </c>
+      <c r="D26" s="15" t="n">
+        <v>644.8</v>
+      </c>
+      <c r="E26" s="6" t="n">
         <v>645</v>
       </c>
-      <c r="D26" s="15" t="n">
-        <v>646.45</v>
-      </c>
-      <c r="E26" s="6" t="n">
-        <v>647.35</v>
-      </c>
       <c r="F26" s="18" t="n">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G26" s="6" t="n">
-        <v>665.15</v>
+        <v>645.85</v>
       </c>
     </row>
     <row r="27">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>248.4</v>
+        <v>252</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>236.3</v>
+        <v>249.05</v>
       </c>
       <c r="D27" s="15" t="n">
-        <v>237.5</v>
+        <v>250</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>238.25</v>
+        <v>249.8</v>
       </c>
       <c r="F27" s="18" t="n">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>247.35</v>
+        <v>251.15</v>
       </c>
     </row>
     <row r="28">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>122.75</v>
+        <v>120.2</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>119.7</v>
+        <v>118.6</v>
       </c>
       <c r="D28" s="15" t="n">
-        <v>120.05</v>
+        <v>119.75</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>120</v>
+        <v>119.65</v>
       </c>
       <c r="F28" s="18" t="n">
-        <v>306</v>
+        <v>258</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>122.5</v>
+        <v>118.8</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" thickBot="1">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B29" s="10" t="n">
-        <v>8523.6</v>
+        <v>8695</v>
       </c>
       <c r="C29" s="13" t="n">
-        <v>8302.549999999999</v>
+        <v>8582.549999999999</v>
       </c>
       <c r="D29" s="16" t="n">
-        <v>8322.549999999999</v>
+        <v>8681</v>
       </c>
       <c r="E29" s="7" t="n">
-        <v>8325.25</v>
+        <v>8685.75</v>
       </c>
       <c r="F29" s="19" t="n">
         <v>2</v>
       </c>
       <c r="G29" s="7" t="n">
-        <v>8459</v>
+        <v>8639.049999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed creation of 1 min sheets with formatting
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -641,7 +641,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1142,7 @@
         <v>245.05</v>
       </c>
       <c r="D22" s="15">
-        <v>2315.1</v>
+        <v>245.7</v>
       </c>
       <c r="E22" s="6">
         <v>245.7</v>
@@ -1165,7 +1165,7 @@
         <v>2311.6999999999998</v>
       </c>
       <c r="D23" s="15">
-        <v>581.29999999999995</v>
+        <v>2315.1</v>
       </c>
       <c r="E23" s="6">
         <v>2314.6</v>
@@ -1188,7 +1188,7 @@
         <v>575.20000000000005</v>
       </c>
       <c r="D24" s="15">
-        <v>672.5</v>
+        <v>581.29999999999995</v>
       </c>
       <c r="E24" s="6">
         <v>581.35</v>
@@ -1211,7 +1211,7 @@
         <v>658.35</v>
       </c>
       <c r="D25" s="15">
-        <v>947.15</v>
+        <v>672.5</v>
       </c>
       <c r="E25" s="6">
         <v>672.25</v>
@@ -1234,7 +1234,7 @@
         <v>945.2</v>
       </c>
       <c r="D26" s="15">
-        <v>653.5</v>
+        <v>947.15</v>
       </c>
       <c r="E26" s="6">
         <v>946.65</v>
@@ -1257,7 +1257,7 @@
         <v>649.5</v>
       </c>
       <c r="D27" s="15">
-        <v>257.35000000000002</v>
+        <v>653.5</v>
       </c>
       <c r="E27" s="6">
         <v>653.25</v>
@@ -1280,7 +1280,7 @@
         <v>252.05</v>
       </c>
       <c r="D28" s="15">
-        <v>120.8</v>
+        <v>257.35000000000002</v>
       </c>
       <c r="E28" s="6">
         <v>257.05</v>
@@ -1303,7 +1303,7 @@
         <v>120.1</v>
       </c>
       <c r="D29" s="15">
-        <v>8678.9</v>
+        <v>120.8</v>
       </c>
       <c r="E29" s="6">
         <v>121</v>
@@ -1326,7 +1326,7 @@
         <v>8660</v>
       </c>
       <c r="D30" s="16">
-        <v>8720</v>
+        <v>8678.9</v>
       </c>
       <c r="E30" s="7">
         <v>8677.4</v>

</xml_diff>

<commit_message>
added weekly to algo data
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="144525" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -598,7 +598,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>2242</v>
+        <v>2232.55</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>2220.5</v>
+        <v>2185.05</v>
       </c>
       <c r="D2" s="14" t="n">
-        <v>2223.95</v>
+        <v>2197.6</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>2225.4</v>
+        <v>2196.65</v>
       </c>
       <c r="F2" s="17" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>2234.7</v>
+        <v>2188.1</v>
       </c>
     </row>
     <row r="3">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>429.15</v>
+        <v>428.6</v>
       </c>
       <c r="C3" s="12" t="n">
-        <v>416</v>
+        <v>423.75</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>427.55</v>
+        <v>424</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>428.3</v>
+        <v>424.6</v>
       </c>
       <c r="F3" s="18" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>417.55</v>
+        <v>426.3</v>
       </c>
     </row>
     <row r="4">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>1615</v>
+        <v>1616.45</v>
       </c>
       <c r="C4" s="12" t="n">
-        <v>1579.95</v>
+        <v>1594.5</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>1586.2</v>
+        <v>1607</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>1587.05</v>
+        <v>1610.4</v>
       </c>
       <c r="F4" s="18" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>1593.15</v>
+        <v>1604.25</v>
       </c>
     </row>
     <row r="5">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>7450</v>
+        <v>7128.85</v>
       </c>
       <c r="C5" s="12" t="n">
-        <v>7119.15</v>
+        <v>7049</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>7216.95</v>
+        <v>7100</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>7224.3</v>
+        <v>7103.15</v>
       </c>
       <c r="F5" s="18" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>7432.65</v>
+        <v>7057.5</v>
       </c>
     </row>
     <row r="6">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>224.3</v>
+        <v>215.2</v>
       </c>
       <c r="C6" s="12" t="n">
-        <v>220.95</v>
+        <v>213.25</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>222.1</v>
+        <v>213.8</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>222.1</v>
+        <v>213.9</v>
       </c>
       <c r="F6" s="18" t="n">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>221.45</v>
+        <v>215.1</v>
       </c>
     </row>
     <row r="7">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>199.35</v>
+        <v>198.45</v>
       </c>
       <c r="C7" s="12" t="n">
-        <v>197.25</v>
+        <v>194.65</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>197.85</v>
+        <v>195.5</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>197.7</v>
+        <v>195.75</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>181</v>
+        <v>89</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>198.75</v>
+        <v>198.05</v>
       </c>
     </row>
     <row r="8">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>354.4</v>
+        <v>338.5</v>
       </c>
       <c r="C8" s="12" t="n">
-        <v>349.5</v>
+        <v>328.85</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>351.15</v>
+        <v>334.4</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>350.6</v>
+        <v>334.2</v>
       </c>
       <c r="F8" s="18" t="n">
-        <v>350</v>
+        <v>151</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>351.15</v>
+        <v>335.4</v>
       </c>
     </row>
     <row r="9">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>624.45</v>
+        <v>641.2</v>
       </c>
       <c r="C9" s="12" t="n">
-        <v>612.25</v>
+        <v>627.15</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>621.75</v>
+        <v>633.35</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>622.1</v>
+        <v>634.45</v>
       </c>
       <c r="F9" s="18" t="n">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>613</v>
+        <v>631.65</v>
       </c>
     </row>
     <row r="10">
@@ -847,22 +847,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>3860</v>
+        <v>3863.8</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>3681.45</v>
+        <v>3826.05</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>3840</v>
+        <v>3835</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>3848.3</v>
+        <v>3844.2</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>3683.6</v>
+        <v>3855</v>
       </c>
     </row>
     <row r="11">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>154.25</v>
+        <v>148.2</v>
       </c>
       <c r="C11" s="12" t="n">
-        <v>149.85</v>
+        <v>146.5</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>150.25</v>
+        <v>146.55</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>150.15</v>
+        <v>146.7</v>
       </c>
       <c r="F11" s="18" t="n">
-        <v>222</v>
+        <v>77</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>154.2</v>
+        <v>147.55</v>
       </c>
     </row>
     <row r="12">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>1283</v>
+        <v>1334.4</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>1270.8</v>
+        <v>1321.8</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>1278.2</v>
+        <v>1326.05</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>1276.65</v>
+        <v>1326.6</v>
       </c>
       <c r="F12" s="18" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>1271.5</v>
+        <v>1331.5</v>
       </c>
     </row>
     <row r="13">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>1510.95</v>
+        <v>1522</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>1501.8</v>
+        <v>1513.4</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>1504.8</v>
+        <v>1518.25</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>1504.4</v>
+        <v>1517.95</v>
       </c>
       <c r="F13" s="18" t="n">
-        <v>206</v>
+        <v>124</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>1510.05</v>
+        <v>1516.75</v>
       </c>
     </row>
     <row r="14">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>513.5</v>
+        <v>510.95</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>502.65</v>
+        <v>505.45</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>505.65</v>
+        <v>506.55</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>505.4</v>
+        <v>506.85</v>
       </c>
       <c r="F14" s="18" t="n">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>511.45</v>
+        <v>505.95</v>
       </c>
     </row>
     <row r="15">
@@ -972,22 +972,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>943.55</v>
+        <v>928.05</v>
       </c>
       <c r="C15" s="12" t="n">
-        <v>939.5</v>
+        <v>922</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>942</v>
+        <v>927.45</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>941.1</v>
+        <v>926.1</v>
       </c>
       <c r="F15" s="18" t="n">
-        <v>194</v>
+        <v>89</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>939.65</v>
+        <v>925.05</v>
       </c>
     </row>
     <row r="16">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1536</v>
+        <v>1507</v>
       </c>
       <c r="C16" s="12" t="n">
-        <v>1490.25</v>
+        <v>1494.1</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>1495</v>
+        <v>1502</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1493.95</v>
+        <v>1502.05</v>
       </c>
       <c r="F16" s="18" t="n">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1535.8</v>
+        <v>1506.15</v>
       </c>
     </row>
     <row r="17">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1414</v>
+        <v>1448.65</v>
       </c>
       <c r="C17" s="12" t="n">
-        <v>1393.05</v>
+        <v>1436.75</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>1412</v>
+        <v>1439.4</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1410.5</v>
+        <v>1439</v>
       </c>
       <c r="F17" s="18" t="n">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1394.5</v>
+        <v>1446.25</v>
       </c>
     </row>
     <row r="18">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>658.2</v>
+        <v>660.5</v>
       </c>
       <c r="C18" s="12" t="n">
-        <v>646.45</v>
+        <v>652.7</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>648</v>
+        <v>654.35</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>648.3</v>
+        <v>654.65</v>
       </c>
       <c r="F18" s="18" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>650.55</v>
+        <v>656</v>
       </c>
     </row>
     <row r="19">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>467.95</v>
+        <v>465.8</v>
       </c>
       <c r="C19" s="12" t="n">
-        <v>457.55</v>
+        <v>460.5</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>466.45</v>
+        <v>461.8</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>466.15</v>
+        <v>462.05</v>
       </c>
       <c r="F19" s="18" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>458.8</v>
+        <v>464.8</v>
       </c>
     </row>
     <row r="20">
@@ -1097,22 +1097,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>1546.4</v>
+        <v>1571.4</v>
       </c>
       <c r="C20" s="12" t="n">
-        <v>1533.55</v>
+        <v>1551.2</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>1541.25</v>
+        <v>1561.25</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>1544.15</v>
+        <v>1559.75</v>
       </c>
       <c r="F20" s="18" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>1538.5</v>
+        <v>1556.4</v>
       </c>
     </row>
     <row r="21">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>279.6</v>
+        <v>276.5</v>
       </c>
       <c r="C21" s="12" t="n">
-        <v>274.65</v>
+        <v>272.4</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>277.25</v>
+        <v>275.15</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>276.4</v>
+        <v>275.15</v>
       </c>
       <c r="F21" s="18" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>276.35</v>
+        <v>275.4</v>
       </c>
     </row>
     <row r="22">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>248.7</v>
+        <v>251.65</v>
       </c>
       <c r="C22" s="12" t="n">
-        <v>246.1</v>
+        <v>247.3</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>247.2</v>
+        <v>249.75</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>247.3</v>
+        <v>250</v>
       </c>
       <c r="F22" s="18" t="n">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>246.95</v>
+        <v>250.55</v>
       </c>
     </row>
     <row r="23">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>2361.95</v>
+        <v>2388</v>
       </c>
       <c r="C23" s="12" t="n">
-        <v>2330.05</v>
+        <v>2364.1</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>2356.1</v>
+        <v>2377</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>2356.45</v>
+        <v>2378.9</v>
       </c>
       <c r="F23" s="18" t="n">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>2330.25</v>
+        <v>2365.55</v>
       </c>
     </row>
     <row r="24">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>586</v>
+        <v>566.2</v>
       </c>
       <c r="C24" s="12" t="n">
-        <v>582.6</v>
+        <v>561</v>
       </c>
       <c r="D24" s="15" t="n">
-        <v>584</v>
+        <v>561.4</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>584.7</v>
+        <v>561.5</v>
       </c>
       <c r="F24" s="18" t="n">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>585.05</v>
+        <v>565.75</v>
       </c>
     </row>
     <row r="25">
@@ -1222,22 +1222,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>670.7</v>
+        <v>676.7</v>
       </c>
       <c r="C25" s="12" t="n">
-        <v>664</v>
+        <v>660.5</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>667.1</v>
+        <v>663.1</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>665.95</v>
+        <v>662.55</v>
       </c>
       <c r="F25" s="18" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>670.65</v>
+        <v>675</v>
       </c>
     </row>
     <row r="26">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>955.55</v>
+        <v>971</v>
       </c>
       <c r="C26" s="12" t="n">
-        <v>948.1</v>
+        <v>960.15</v>
       </c>
       <c r="D26" s="15" t="n">
-        <v>949.5</v>
+        <v>963.3</v>
       </c>
       <c r="E26" s="6" t="n">
-        <v>949.55</v>
+        <v>961.3</v>
       </c>
       <c r="F26" s="18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G26" s="6" t="n">
-        <v>951.6</v>
+        <v>962</v>
       </c>
     </row>
     <row r="27">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>673.5</v>
+        <v>683.3</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>656.55</v>
+        <v>675.25</v>
       </c>
       <c r="D27" s="15" t="n">
-        <v>671.5</v>
+        <v>681</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>671.55</v>
+        <v>681.7</v>
       </c>
       <c r="F27" s="18" t="n">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>657.55</v>
+        <v>677.4</v>
       </c>
     </row>
     <row r="28">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>262.25</v>
+        <v>263.85</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>258.35</v>
+        <v>260.75</v>
       </c>
       <c r="D28" s="15" t="n">
-        <v>259.1</v>
+        <v>262.6</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>259.2</v>
+        <v>262.65</v>
       </c>
       <c r="F28" s="18" t="n">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>259.05</v>
+        <v>263.55</v>
       </c>
     </row>
     <row r="29">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B29" s="9" t="n">
-        <v>124.4</v>
+        <v>126.4</v>
       </c>
       <c r="C29" s="12" t="n">
-        <v>122.4</v>
+        <v>125.55</v>
       </c>
       <c r="D29" s="15" t="n">
-        <v>124.1</v>
+        <v>126.2</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>124.05</v>
+        <v>126.25</v>
       </c>
       <c r="F29" s="18" t="n">
-        <v>383</v>
+        <v>296</v>
       </c>
       <c r="G29" s="6" t="n">
-        <v>123.25</v>
+        <v>125.75</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1" thickBot="1">
@@ -1347,22 +1347,22 @@
         </is>
       </c>
       <c r="B30" s="10" t="n">
-        <v>8815.75</v>
+        <v>8724.35</v>
       </c>
       <c r="C30" s="13" t="n">
-        <v>8721</v>
+        <v>8665</v>
       </c>
       <c r="D30" s="16" t="n">
-        <v>8747.6</v>
+        <v>8704</v>
       </c>
       <c r="E30" s="7" t="n">
-        <v>8766.9</v>
+        <v>8708.35</v>
       </c>
       <c r="F30" s="19" t="n">
         <v>1</v>
       </c>
       <c r="G30" s="7" t="n">
-        <v>8730</v>
+        <v>8717.950000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
potential fix for color checking issue
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>634.5</v>
+        <v>633.65</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>615.35</v>
+        <v>624.65</v>
       </c>
       <c r="D2" s="14" t="n">
-        <v>627</v>
+        <v>627.3</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>628.35</v>
+        <v>628</v>
       </c>
       <c r="F2" s="17" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>621.9</v>
+        <v>625</v>
       </c>
     </row>
     <row r="3">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>3066.9</v>
+        <v>3322.9</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>2974.95</v>
+        <v>3225</v>
       </c>
       <c r="D3" s="14" t="n">
-        <v>3034.05</v>
+        <v>3255</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>3041.65</v>
+        <v>3258.8</v>
       </c>
       <c r="F3" s="17" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>3056.95</v>
+        <v>3234.85</v>
       </c>
     </row>
     <row r="4">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>508.3</v>
+        <v>471.85</v>
       </c>
       <c r="C4" s="12" t="n">
-        <v>482.25</v>
+        <v>467.1</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>489</v>
+        <v>471.35</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>488.15</v>
+        <v>471.05</v>
       </c>
       <c r="F4" s="18" t="n">
-        <v>155</v>
+        <v>24</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>501.55</v>
+        <v>468.2</v>
       </c>
     </row>
     <row r="5">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>1601</v>
+        <v>1595.75</v>
       </c>
       <c r="C5" s="12" t="n">
-        <v>1560.45</v>
+        <v>1565.1</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>1593.95</v>
+        <v>1567.05</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>1596</v>
+        <v>1569.9</v>
       </c>
       <c r="F5" s="18" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>1572.7</v>
+        <v>1595.7</v>
       </c>
     </row>
     <row r="6">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>6762.1</v>
+        <v>6894</v>
       </c>
       <c r="C6" s="12" t="n">
-        <v>6623.05</v>
+        <v>6785.35</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>6731</v>
+        <v>6791.65</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>6747.15</v>
+        <v>6806.7</v>
       </c>
       <c r="F6" s="18" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>6705</v>
+        <v>6870.1</v>
       </c>
     </row>
     <row r="7">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>185.45</v>
+        <v>194.1</v>
       </c>
       <c r="C7" s="12" t="n">
-        <v>176.55</v>
+        <v>189.5</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>180.2</v>
+        <v>191.6</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>179.6</v>
+        <v>191.7</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>400</v>
+        <v>113</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>185</v>
+        <v>189.7</v>
       </c>
     </row>
     <row r="8">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>267.1</v>
+        <v>266.2</v>
       </c>
       <c r="C8" s="12" t="n">
-        <v>259.05</v>
+        <v>262.55</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>263.8</v>
+        <v>263.5</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>262.9</v>
+        <v>263.4</v>
       </c>
       <c r="F8" s="18" t="n">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>265.95</v>
+        <v>263.75</v>
       </c>
     </row>
     <row r="9">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>475</v>
+        <v>491.9</v>
       </c>
       <c r="C9" s="12" t="n">
-        <v>457.85</v>
+        <v>485</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>467.25</v>
+        <v>486.1</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>468.3</v>
+        <v>486.45</v>
       </c>
       <c r="F9" s="18" t="n">
-        <v>172</v>
+        <v>80</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>468.1</v>
+        <v>486.15</v>
       </c>
     </row>
     <row r="10">
@@ -847,22 +847,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>846.35</v>
+        <v>825.9</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>826.35</v>
+        <v>816.55</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>845.05</v>
+        <v>819</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>841.5</v>
+        <v>818.3</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>832.15</v>
+        <v>817.95</v>
       </c>
     </row>
     <row r="11">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>4695.55</v>
+        <v>4808.85</v>
       </c>
       <c r="C11" s="12" t="n">
-        <v>4543.1</v>
+        <v>4734</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>4663.05</v>
+        <v>4757.25</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>4681.75</v>
+        <v>4745.4</v>
       </c>
       <c r="F11" s="18" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>4665.1</v>
+        <v>4755.6</v>
       </c>
     </row>
     <row r="12">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>164.8</v>
+        <v>160.9</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>161.7</v>
+        <v>158.95</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>164.5</v>
+        <v>160.15</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>164.1</v>
+        <v>159.5</v>
       </c>
       <c r="F12" s="18" t="n">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>163.2</v>
+        <v>159.65</v>
       </c>
     </row>
     <row r="13">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>1357.8</v>
+        <v>1360.95</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>1328.5</v>
+        <v>1346.95</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>1347.15</v>
+        <v>1347.95</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>1348.15</v>
+        <v>1353.1</v>
       </c>
       <c r="F13" s="18" t="n">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>1352.8</v>
+        <v>1360.6</v>
       </c>
     </row>
     <row r="14">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>1462.55</v>
+        <v>1520.4</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>1435.5</v>
+        <v>1501.25</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>1459.75</v>
+        <v>1506</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>1460.25</v>
+        <v>1508.3</v>
       </c>
       <c r="F14" s="18" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>1446.1</v>
+        <v>1520.05</v>
       </c>
     </row>
     <row r="15">
@@ -972,22 +972,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>666</v>
+        <v>713.5</v>
       </c>
       <c r="C15" s="12" t="n">
-        <v>643.25</v>
+        <v>684.4</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>652.3</v>
+        <v>705.3</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>653.35</v>
+        <v>705.3</v>
       </c>
       <c r="F15" s="18" t="n">
-        <v>87</v>
+        <v>226</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>663.9</v>
+        <v>689.2</v>
       </c>
     </row>
     <row r="16">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1136.1</v>
+        <v>1120.35</v>
       </c>
       <c r="C16" s="12" t="n">
-        <v>1112.8</v>
+        <v>1098.5</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>1129</v>
+        <v>1104</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1131.05</v>
+        <v>1102</v>
       </c>
       <c r="F16" s="18" t="n">
-        <v>142</v>
+        <v>192</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1135.2</v>
+        <v>1119.55</v>
       </c>
     </row>
     <row r="17">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1415.7</v>
+        <v>1470.55</v>
       </c>
       <c r="C17" s="12" t="n">
-        <v>1385.65</v>
+        <v>1439.25</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>1410</v>
+        <v>1463.45</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1408.75</v>
+        <v>1460.25</v>
       </c>
       <c r="F17" s="18" t="n">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1415.5</v>
+        <v>1444.9</v>
       </c>
     </row>
     <row r="18">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>1455.75</v>
+        <v>1462.25</v>
       </c>
       <c r="C18" s="12" t="n">
-        <v>1433.2</v>
+        <v>1450</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>1450.9</v>
+        <v>1455</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>1453.35</v>
+        <v>1450.95</v>
       </c>
       <c r="F18" s="18" t="n">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>1446</v>
+        <v>1460.9</v>
       </c>
     </row>
     <row r="19">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>1009.95</v>
+        <v>1051.15</v>
       </c>
       <c r="C19" s="12" t="n">
-        <v>994.05</v>
+        <v>1030.25</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>1005.5</v>
+        <v>1037.75</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>1005.25</v>
+        <v>1038.55</v>
       </c>
       <c r="F19" s="18" t="n">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>1005.35</v>
+        <v>1048.7</v>
       </c>
     </row>
     <row r="20">
@@ -1097,22 +1097,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>657.15</v>
+        <v>653.85</v>
       </c>
       <c r="C20" s="12" t="n">
-        <v>625</v>
+        <v>642.45</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>655.8</v>
+        <v>645</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>653.15</v>
+        <v>646.8</v>
       </c>
       <c r="F20" s="18" t="n">
-        <v>121</v>
+        <v>20</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>633.45</v>
+        <v>643.3</v>
       </c>
     </row>
     <row r="21">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>2393.9</v>
+        <v>2547</v>
       </c>
       <c r="C21" s="12" t="n">
-        <v>2286.2</v>
+        <v>2500.95</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>2393.9</v>
+        <v>2530</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>2371.75</v>
+        <v>2533.65</v>
       </c>
       <c r="F21" s="18" t="n">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>2330.05</v>
+        <v>2517.5</v>
       </c>
     </row>
     <row r="22">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>268.3</v>
+        <v>270.6</v>
       </c>
       <c r="C22" s="12" t="n">
-        <v>264.75</v>
+        <v>267.25</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>267.75</v>
+        <v>267.65</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>266.65</v>
+        <v>268.45</v>
       </c>
       <c r="F22" s="18" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>267</v>
+        <v>268.55</v>
       </c>
     </row>
     <row r="23">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>362.1</v>
+        <v>366.35</v>
       </c>
       <c r="C23" s="12" t="n">
-        <v>353.05</v>
+        <v>361.5</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>361.45</v>
+        <v>364.6</v>
       </c>
       <c r="F23" s="18" t="n">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>360.35</v>
+        <v>362.5</v>
       </c>
     </row>
     <row r="24">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>2855</v>
+        <v>2916</v>
       </c>
       <c r="C24" s="12" t="n">
-        <v>2796.05</v>
+        <v>2876.9</v>
       </c>
       <c r="D24" s="15" t="n">
-        <v>2851</v>
+        <v>2881.05</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>2850.7</v>
+        <v>2881.55</v>
       </c>
       <c r="F24" s="18" t="n">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>2844.1</v>
+        <v>2906.55</v>
       </c>
     </row>
     <row r="25">
@@ -1222,22 +1222,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>825.8</v>
+        <v>834.45</v>
       </c>
       <c r="C25" s="12" t="n">
-        <v>797.35</v>
+        <v>819.3</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>812.3</v>
+        <v>825</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>811.95</v>
+        <v>822.65</v>
       </c>
       <c r="F25" s="18" t="n">
-        <v>205</v>
+        <v>145</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>825</v>
+        <v>830.7</v>
       </c>
     </row>
     <row r="26">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>672.35</v>
+        <v>668.95</v>
       </c>
       <c r="C26" s="12" t="n">
-        <v>661.45</v>
+        <v>651.15</v>
       </c>
       <c r="D26" s="15" t="n">
-        <v>668.75</v>
+        <v>654</v>
       </c>
       <c r="E26" s="6" t="n">
-        <v>670</v>
+        <v>653.75</v>
       </c>
       <c r="F26" s="18" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G26" s="6" t="n">
-        <v>662.75</v>
+        <v>657</v>
       </c>
     </row>
     <row r="27">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>1085</v>
+        <v>1101.45</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>1071.4</v>
+        <v>1070.25</v>
       </c>
       <c r="D27" s="15" t="n">
-        <v>1082</v>
+        <v>1072.7</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>1083</v>
+        <v>1072.3</v>
       </c>
       <c r="F27" s="18" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>1080.05</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="28">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>942.85</v>
+        <v>950.5</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>919</v>
+        <v>939.8</v>
       </c>
       <c r="D28" s="15" t="n">
-        <v>939.2</v>
+        <v>943.5</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>936.4</v>
+        <v>943.6</v>
       </c>
       <c r="F28" s="18" t="n">
-        <v>312</v>
+        <v>81</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>940.2</v>
+        <v>941.85</v>
       </c>
     </row>
     <row r="29">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B29" s="9" t="n">
-        <v>435</v>
+        <v>439.45</v>
       </c>
       <c r="C29" s="12" t="n">
-        <v>426.85</v>
+        <v>432.1</v>
       </c>
       <c r="D29" s="15" t="n">
-        <v>434.55</v>
+        <v>433.5</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>433.95</v>
+        <v>432.85</v>
       </c>
       <c r="F29" s="18" t="n">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G29" s="6" t="n">
-        <v>430.45</v>
+        <v>436</v>
       </c>
     </row>
     <row r="30">
@@ -1347,22 +1347,22 @@
         </is>
       </c>
       <c r="B30" s="9" t="n">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="C30" s="12" t="n">
-        <v>162.3</v>
+        <v>173.5</v>
       </c>
       <c r="D30" s="15" t="n">
-        <v>165.85</v>
+        <v>174</v>
       </c>
       <c r="E30" s="6" t="n">
-        <v>165.9</v>
+        <v>174.25</v>
       </c>
       <c r="F30" s="18" t="n">
-        <v>411</v>
+        <v>365</v>
       </c>
       <c r="G30" s="6" t="n">
-        <v>167.8</v>
+        <v>175.25</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" thickBot="1">
@@ -1372,22 +1372,22 @@
         </is>
       </c>
       <c r="B31" s="10" t="n">
-        <v>9725.700000000001</v>
+        <v>10169.95</v>
       </c>
       <c r="C31" s="13" t="n">
-        <v>9525.5</v>
+        <v>9961</v>
       </c>
       <c r="D31" s="16" t="n">
-        <v>9700</v>
+        <v>10031</v>
       </c>
       <c r="E31" s="7" t="n">
-        <v>9709.1</v>
+        <v>10023.4</v>
       </c>
       <c r="F31" s="19" t="n">
         <v>3</v>
       </c>
       <c r="G31" s="7" t="n">
-        <v>9608.4</v>
+        <v>10141.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ongc and bhel in algo and changed shares in 30 min
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>720.35</v>
+        <v>640.2</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>703.8</v>
+        <v>622.3</v>
       </c>
       <c r="D2" s="14" t="n">
-        <v>708.1</v>
+        <v>628.2</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>708.4</v>
+        <v>628.7</v>
       </c>
       <c r="F2" s="17" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>719.2</v>
+        <v>635</v>
       </c>
     </row>
     <row r="3">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>3143.55</v>
+        <v>3038</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>3075</v>
+        <v>2981.3</v>
       </c>
       <c r="D3" s="14" t="n">
-        <v>3112</v>
+        <v>3022</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>3113.6</v>
+        <v>3020.15</v>
       </c>
       <c r="F3" s="17" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>3139.4</v>
+        <v>3034.95</v>
       </c>
     </row>
     <row r="4">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>533.5</v>
+        <v>500.5</v>
       </c>
       <c r="C4" s="12" t="n">
-        <v>520</v>
+        <v>485</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>523.7</v>
+        <v>493.1</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>522.35</v>
+        <v>492.35</v>
       </c>
       <c r="F4" s="18" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>527.95</v>
+        <v>498.6</v>
       </c>
     </row>
     <row r="5">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>1574.5</v>
+        <v>1772</v>
       </c>
       <c r="C5" s="12" t="n">
-        <v>1562</v>
+        <v>1715.9</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>1568</v>
+        <v>1758.3</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>1570.1</v>
+        <v>1755.65</v>
       </c>
       <c r="F5" s="18" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>1573.35</v>
+        <v>1718.55</v>
       </c>
     </row>
     <row r="6">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>7108</v>
+        <v>7158</v>
       </c>
       <c r="C6" s="12" t="n">
-        <v>7047</v>
+        <v>6893.2</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>7099</v>
+        <v>7066.65</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>7098.25</v>
+        <v>7063.55</v>
       </c>
       <c r="F6" s="18" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>7100</v>
+        <v>6895.05</v>
       </c>
     </row>
     <row r="7">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>205.22</v>
+        <v>196.5</v>
       </c>
       <c r="C7" s="12" t="n">
-        <v>201.5</v>
+        <v>191.64</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>204</v>
+        <v>194.22</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>204.47</v>
+        <v>193.93</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>87</v>
+        <v>212</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>202.85</v>
+        <v>196.27</v>
       </c>
     </row>
     <row r="8">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>266.8</v>
+        <v>250.7</v>
       </c>
       <c r="C8" s="12" t="n">
-        <v>261.55</v>
+        <v>247.65</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>263</v>
+        <v>250.1</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>262.35</v>
+        <v>249.8</v>
       </c>
       <c r="F8" s="18" t="n">
-        <v>228</v>
+        <v>99</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>263.55</v>
+        <v>249.65</v>
       </c>
     </row>
     <row r="9">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>496</v>
+        <v>530</v>
       </c>
       <c r="C9" s="12" t="n">
-        <v>487.2</v>
+        <v>516.1</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>493.5</v>
+        <v>529.15</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>493.3</v>
+        <v>527.55</v>
       </c>
       <c r="F9" s="18" t="n">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>490.7</v>
+        <v>525.35</v>
       </c>
     </row>
     <row r="10">
@@ -847,22 +847,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>839.1</v>
+        <v>835.35</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>828.05</v>
+        <v>818.5</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>834.2</v>
+        <v>835.2</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>835.7</v>
+        <v>831.9</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>838.5</v>
+        <v>834.05</v>
       </c>
     </row>
     <row r="11">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>4775</v>
+        <v>4994.4</v>
       </c>
       <c r="C11" s="12" t="n">
-        <v>4716</v>
+        <v>4880</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>4752.55</v>
+        <v>4902.65</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>4754.45</v>
+        <v>4915.9</v>
       </c>
       <c r="F11" s="18" t="n">
         <v>5</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>4751.7</v>
+        <v>4945</v>
       </c>
     </row>
     <row r="12">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>189.3</v>
+        <v>196.88</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>185.27</v>
+        <v>194.5</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>188.3</v>
+        <v>195.99</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>188.06</v>
+        <v>195.92</v>
       </c>
       <c r="F12" s="18" t="n">
-        <v>174</v>
+        <v>55</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>187.06</v>
+        <v>195.28</v>
       </c>
     </row>
     <row r="13">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>1540</v>
+        <v>1756</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>1506.2</v>
+        <v>1707.55</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>1537.95</v>
+        <v>1750.45</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>1533.4</v>
+        <v>1751.85</v>
       </c>
       <c r="F13" s="18" t="n">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>1524.6</v>
+        <v>1709.4</v>
       </c>
     </row>
     <row r="14">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>1654.95</v>
+        <v>1644.4</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>1627.15</v>
+        <v>1631.15</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>1636.35</v>
+        <v>1639.95</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>1635.35</v>
+        <v>1638.55</v>
       </c>
       <c r="F14" s="18" t="n">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>1653.2</v>
+        <v>1644.15</v>
       </c>
     </row>
     <row r="15">
@@ -972,22 +972,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>705.9</v>
+        <v>702.35</v>
       </c>
       <c r="C15" s="12" t="n">
-        <v>691.65</v>
+        <v>691.4</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>697.6</v>
+        <v>700</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>697.2</v>
+        <v>700.5</v>
       </c>
       <c r="F15" s="18" t="n">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>700.8</v>
+        <v>695.8</v>
       </c>
     </row>
     <row r="16">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1239.5</v>
+        <v>1235</v>
       </c>
       <c r="C16" s="12" t="n">
-        <v>1226.05</v>
+        <v>1218.9</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>1237</v>
+        <v>1222.75</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1235.05</v>
+        <v>1221.9</v>
       </c>
       <c r="F16" s="18" t="n">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1233.7</v>
+        <v>1222.8</v>
       </c>
     </row>
     <row r="17">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1441.7</v>
+        <v>1423.05</v>
       </c>
       <c r="C17" s="12" t="n">
-        <v>1426.3</v>
+        <v>1407.8</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>1439</v>
+        <v>1415.5</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1438.05</v>
+        <v>1417.45</v>
       </c>
       <c r="F17" s="18" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1435.6</v>
+        <v>1413.4</v>
       </c>
     </row>
     <row r="18">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>1666</v>
+        <v>1950.5</v>
       </c>
       <c r="C18" s="12" t="n">
-        <v>1648</v>
+        <v>1920.9</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>1660.95</v>
+        <v>1930.2</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>1661.65</v>
+        <v>1933.35</v>
       </c>
       <c r="F18" s="18" t="n">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>1653.4</v>
+        <v>1929.05</v>
       </c>
     </row>
     <row r="19">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>1050.4</v>
+        <v>967</v>
       </c>
       <c r="C19" s="12" t="n">
-        <v>1023.5</v>
+        <v>948.55</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>1027</v>
+        <v>961</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>1025.95</v>
+        <v>960.5</v>
       </c>
       <c r="F19" s="18" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>1048.5</v>
+        <v>962.35</v>
       </c>
     </row>
     <row r="20">
@@ -1097,22 +1097,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>792.05</v>
+        <v>681.9</v>
       </c>
       <c r="C20" s="12" t="n">
-        <v>780.2</v>
+        <v>667.05</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>783.8</v>
+        <v>677.75</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>782.15</v>
+        <v>675.95</v>
       </c>
       <c r="F20" s="18" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>787.6</v>
+        <v>676.95</v>
       </c>
     </row>
     <row r="21">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>2918.6</v>
+        <v>2801.65</v>
       </c>
       <c r="C21" s="12" t="n">
-        <v>2847.5</v>
+        <v>2741.65</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>2849.65</v>
+        <v>2763</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>2851.35</v>
+        <v>2757.6</v>
       </c>
       <c r="F21" s="18" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>2898.5</v>
+        <v>2791</v>
       </c>
     </row>
     <row r="22">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>305.35</v>
+        <v>317.8</v>
       </c>
       <c r="C22" s="12" t="n">
-        <v>298</v>
+        <v>308.9</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>303.5</v>
+        <v>314.7</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>302.8</v>
+        <v>313.4</v>
       </c>
       <c r="F22" s="18" t="n">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>299.65</v>
+        <v>315.75</v>
       </c>
     </row>
     <row r="23">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>380.7</v>
+        <v>412.6</v>
       </c>
       <c r="C23" s="12" t="n">
-        <v>376.15</v>
+        <v>403.75</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>378.1</v>
+        <v>411.1</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>377.45</v>
+        <v>409.9</v>
       </c>
       <c r="F23" s="18" t="n">
-        <v>88</v>
+        <v>190</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>378.7</v>
+        <v>410.5</v>
       </c>
     </row>
     <row r="24">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>3217.6</v>
+        <v>3074</v>
       </c>
       <c r="C24" s="12" t="n">
-        <v>3165.05</v>
+        <v>2988</v>
       </c>
       <c r="D24" s="15" t="n">
-        <v>3201.5</v>
+        <v>3042.9</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>3201.8</v>
+        <v>3041.85</v>
       </c>
       <c r="F24" s="18" t="n">
-        <v>47</v>
+        <v>191</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>3182.05</v>
+        <v>2997.15</v>
       </c>
     </row>
     <row r="25">
@@ -1222,22 +1222,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>865</v>
+        <v>816</v>
       </c>
       <c r="C25" s="12" t="n">
-        <v>854.65</v>
+        <v>809.1</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>856.75</v>
+        <v>815.7</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>856.25</v>
+        <v>814.5</v>
       </c>
       <c r="F25" s="18" t="n">
-        <v>103</v>
+        <v>182</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>859.5</v>
+        <v>810.4</v>
       </c>
     </row>
     <row r="26">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>785.9</v>
+        <v>815.95</v>
       </c>
       <c r="C26" s="12" t="n">
-        <v>771.15</v>
+        <v>800.55</v>
       </c>
       <c r="D26" s="15" t="n">
-        <v>783</v>
+        <v>810.65</v>
       </c>
       <c r="E26" s="6" t="n">
-        <v>784.1</v>
+        <v>809.9</v>
       </c>
       <c r="F26" s="18" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G26" s="6" t="n">
-        <v>781.2</v>
+        <v>814.05</v>
       </c>
     </row>
     <row r="27">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>1111.15</v>
+        <v>1076.55</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>1078.65</v>
+        <v>1057.55</v>
       </c>
       <c r="D27" s="15" t="n">
-        <v>1080.9</v>
+        <v>1072</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>1079.95</v>
+        <v>1073.3</v>
       </c>
       <c r="F27" s="18" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>1102.7</v>
+        <v>1073.85</v>
       </c>
     </row>
     <row r="28">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>1016.6</v>
+        <v>1142</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>996.2</v>
+        <v>1066</v>
       </c>
       <c r="D28" s="15" t="n">
-        <v>1002.9</v>
+        <v>1112.9</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>1002.6</v>
+        <v>1121.65</v>
       </c>
       <c r="F28" s="18" t="n">
-        <v>133</v>
+        <v>406</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>1010.7</v>
+        <v>1076.25</v>
       </c>
     </row>
     <row r="29">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B29" s="9" t="n">
-        <v>442.85</v>
+        <v>433.1</v>
       </c>
       <c r="C29" s="12" t="n">
-        <v>431.9</v>
+        <v>424.7</v>
       </c>
       <c r="D29" s="15" t="n">
-        <v>434</v>
+        <v>430.9</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>433.45</v>
+        <v>430.9</v>
       </c>
       <c r="F29" s="18" t="n">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G29" s="6" t="n">
-        <v>441.95</v>
+        <v>430.4</v>
       </c>
     </row>
     <row r="30">
@@ -1347,22 +1347,22 @@
         </is>
       </c>
       <c r="B30" s="9" t="n">
-        <v>175.47</v>
+        <v>153.56</v>
       </c>
       <c r="C30" s="12" t="n">
-        <v>172.09</v>
+        <v>151.2</v>
       </c>
       <c r="D30" s="15" t="n">
-        <v>172.49</v>
+        <v>153.15</v>
       </c>
       <c r="E30" s="6" t="n">
-        <v>172.28</v>
+        <v>152.97</v>
       </c>
       <c r="F30" s="18" t="n">
-        <v>314</v>
+        <v>444</v>
       </c>
       <c r="G30" s="6" t="n">
-        <v>175.04</v>
+        <v>152.85</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" thickBot="1">
@@ -1372,22 +1372,22 @@
         </is>
       </c>
       <c r="B31" s="10" t="n">
-        <v>11645</v>
+        <v>11256.7</v>
       </c>
       <c r="C31" s="13" t="n">
-        <v>11530</v>
+        <v>11115.4</v>
       </c>
       <c r="D31" s="16" t="n">
-        <v>11579</v>
+        <v>11210</v>
       </c>
       <c r="E31" s="7" t="n">
-        <v>11582.9</v>
+        <v>11222</v>
       </c>
       <c r="F31" s="19" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G31" s="7" t="n">
-        <v>11627.45</v>
+        <v>11141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed share names in cash
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>632.45</v>
+        <v>621.95</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>626.1</v>
+        <v>612.3</v>
       </c>
       <c r="D2" s="14" t="n">
-        <v>628</v>
+        <v>617.9</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>627.05</v>
+        <v>617.05</v>
       </c>
       <c r="F2" s="17" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>630.45</v>
+        <v>613.1</v>
       </c>
     </row>
     <row r="3">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>3035.65</v>
+        <v>3037.9</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>3003.3</v>
+        <v>3002</v>
       </c>
       <c r="D3" s="14" t="n">
-        <v>3033</v>
+        <v>3012</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>3019.35</v>
+        <v>3015.35</v>
       </c>
       <c r="F3" s="17" t="n">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>3018.25</v>
+        <v>3013.75</v>
       </c>
     </row>
     <row r="4">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>498.7</v>
+        <v>515.5</v>
       </c>
       <c r="C4" s="12" t="n">
-        <v>491.6</v>
+        <v>509.5</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>493.5</v>
+        <v>511.3</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>492.9</v>
+        <v>512</v>
       </c>
       <c r="F4" s="18" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>495.25</v>
+        <v>510.15</v>
       </c>
     </row>
     <row r="5">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>1793.5</v>
+        <v>1874.7</v>
       </c>
       <c r="C5" s="12" t="n">
-        <v>1750.05</v>
+        <v>1850</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>1782</v>
+        <v>1865.1</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>1783.05</v>
+        <v>1864.95</v>
       </c>
       <c r="F5" s="18" t="n">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>1777</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="6">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>7215.05</v>
+        <v>7286.65</v>
       </c>
       <c r="C6" s="12" t="n">
-        <v>7100.1</v>
+        <v>7193</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>7210</v>
+        <v>7235</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>7200.15</v>
+        <v>7244.9</v>
       </c>
       <c r="F6" s="18" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>7124.8</v>
+        <v>7275.5</v>
       </c>
     </row>
     <row r="7">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>201.92</v>
+        <v>208.25</v>
       </c>
       <c r="C7" s="12" t="n">
-        <v>196.52</v>
+        <v>202.51</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>201.1</v>
+        <v>203.7</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>200.3</v>
+        <v>203.66</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>1098</v>
+        <v>273</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>196.97</v>
+        <v>202.67</v>
       </c>
     </row>
     <row r="8">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>253.85</v>
+        <v>244.45</v>
       </c>
       <c r="C8" s="12" t="n">
-        <v>249.65</v>
+        <v>240.85</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>249.85</v>
+        <v>244.05</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>250.1</v>
+        <v>243.85</v>
       </c>
       <c r="F8" s="18" t="n">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>251.45</v>
+        <v>242.75</v>
       </c>
     </row>
     <row r="9">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>534.5</v>
+        <v>505.2</v>
       </c>
       <c r="C9" s="12" t="n">
-        <v>522</v>
+        <v>495.15</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>523.95</v>
+        <v>497.2</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>524.95</v>
+        <v>497</v>
       </c>
       <c r="F9" s="18" t="n">
-        <v>309</v>
+        <v>108</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>533.7</v>
+        <v>502.55</v>
       </c>
     </row>
     <row r="10">
@@ -847,22 +847,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>849.55</v>
+        <v>851.8</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>838.65</v>
+        <v>840.15</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>846.05</v>
+        <v>841.5</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>845.1</v>
+        <v>841.65</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>840.5</v>
+        <v>850.6</v>
       </c>
     </row>
     <row r="11">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>4979.5</v>
+        <v>4854.55</v>
       </c>
       <c r="C11" s="12" t="n">
-        <v>4918.05</v>
+        <v>4787.15</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>4956.25</v>
+        <v>4800</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>4960.5</v>
+        <v>4800.1</v>
       </c>
       <c r="F11" s="18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>4931.5</v>
+        <v>4848.45</v>
       </c>
     </row>
     <row r="12">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>198.23</v>
+        <v>190.68</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>194.2</v>
+        <v>187.61</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>195.4</v>
+        <v>190</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>194.7</v>
+        <v>189.65</v>
       </c>
       <c r="F12" s="18" t="n">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>196.71</v>
+        <v>188.28</v>
       </c>
     </row>
     <row r="13">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>1766.3</v>
+        <v>1797.7</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>1742.2</v>
+        <v>1767.3</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>1749.1</v>
+        <v>1794.6</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>1753.25</v>
+        <v>1790.55</v>
       </c>
       <c r="F13" s="18" t="n">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>1758.85</v>
+        <v>1780.05</v>
       </c>
     </row>
     <row r="14">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>1656.3</v>
+        <v>1649.5</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>1621.15</v>
+        <v>1642</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>1625.75</v>
+        <v>1644.4</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>1636.9</v>
+        <v>1645.45</v>
       </c>
       <c r="F14" s="18" t="n">
-        <v>2226</v>
+        <v>114</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>1655.2</v>
+        <v>1648.25</v>
       </c>
     </row>
     <row r="15">
@@ -972,22 +972,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>708.5</v>
+        <v>672.4</v>
       </c>
       <c r="C15" s="12" t="n">
-        <v>695.1</v>
+        <v>667.25</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>700.3</v>
+        <v>669.3</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>701.35</v>
+        <v>669.95</v>
       </c>
       <c r="F15" s="18" t="n">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>695.5</v>
+        <v>669.05</v>
       </c>
     </row>
     <row r="16">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1235.55</v>
+        <v>1241.85</v>
       </c>
       <c r="C16" s="12" t="n">
-        <v>1218.9</v>
+        <v>1231.3</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>1232</v>
+        <v>1235.35</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1229.2</v>
+        <v>1235.95</v>
       </c>
       <c r="F16" s="18" t="n">
-        <v>212</v>
+        <v>91</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1223.5</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="17">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1430</v>
+        <v>1440.55</v>
       </c>
       <c r="C17" s="12" t="n">
-        <v>1415.55</v>
+        <v>1418.9</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>1427.45</v>
+        <v>1426.2</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1425.25</v>
+        <v>1422.9</v>
       </c>
       <c r="F17" s="18" t="n">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1416.45</v>
+        <v>1435.85</v>
       </c>
     </row>
     <row r="18">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>1950</v>
+        <v>1940</v>
       </c>
       <c r="C18" s="12" t="n">
-        <v>1928</v>
+        <v>1909.6</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>1949.85</v>
+        <v>1933</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>1943.7</v>
+        <v>1933.15</v>
       </c>
       <c r="F18" s="18" t="n">
-        <v>134</v>
+        <v>40</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>1934.15</v>
+        <v>1926.9</v>
       </c>
     </row>
     <row r="19">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>976</v>
+        <v>955.65</v>
       </c>
       <c r="C19" s="12" t="n">
-        <v>962.5</v>
+        <v>942.6</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>967.9</v>
+        <v>949.8</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>970.4</v>
+        <v>950.5</v>
       </c>
       <c r="F19" s="18" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>962.95</v>
+        <v>950</v>
       </c>
     </row>
     <row r="20">
@@ -1097,22 +1097,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>682</v>
+        <v>719.5</v>
       </c>
       <c r="C20" s="12" t="n">
-        <v>673.25</v>
+        <v>700.6</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>674.15</v>
+        <v>707.75</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>674.4</v>
+        <v>707.4</v>
       </c>
       <c r="F20" s="18" t="n">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>679</v>
+        <v>703.25</v>
       </c>
     </row>
     <row r="21">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>2821.55</v>
+        <v>2746.55</v>
       </c>
       <c r="C21" s="12" t="n">
-        <v>2765</v>
+        <v>2711.9</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>2812</v>
+        <v>2721</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>2805.4</v>
+        <v>2723.1</v>
       </c>
       <c r="F21" s="18" t="n">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>2773.2</v>
+        <v>2745.9</v>
       </c>
     </row>
     <row r="22">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>317.2</v>
+        <v>332.3</v>
       </c>
       <c r="C22" s="12" t="n">
-        <v>313.5</v>
+        <v>326</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>313.65</v>
+        <v>328.5</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>314.35</v>
+        <v>329.1</v>
       </c>
       <c r="F22" s="18" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>315.45</v>
+        <v>328.45</v>
       </c>
     </row>
     <row r="23">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>419.2</v>
+        <v>408.4</v>
       </c>
       <c r="C23" s="12" t="n">
-        <v>411.5</v>
+        <v>401.85</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>417.2</v>
+        <v>403</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>416.2</v>
+        <v>403.25</v>
       </c>
       <c r="F23" s="18" t="n">
-        <v>226</v>
+        <v>142</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>412.95</v>
+        <v>405.05</v>
       </c>
     </row>
     <row r="24">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>3056</v>
+        <v>3041</v>
       </c>
       <c r="C24" s="12" t="n">
-        <v>3006.65</v>
+        <v>2974.1</v>
       </c>
       <c r="D24" s="15" t="n">
-        <v>3024.95</v>
+        <v>2991</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>3019.25</v>
+        <v>2985.95</v>
       </c>
       <c r="F24" s="18" t="n">
-        <v>208</v>
+        <v>81</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>3051.95</v>
+        <v>3039.65</v>
       </c>
     </row>
     <row r="25">
@@ -1222,22 +1222,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>820.7</v>
+        <v>822.15</v>
       </c>
       <c r="C25" s="12" t="n">
-        <v>814.35</v>
+        <v>815.6</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>816.25</v>
+        <v>818</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>815.6</v>
+        <v>818.75</v>
       </c>
       <c r="F25" s="18" t="n">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>816.5</v>
+        <v>816.35</v>
       </c>
     </row>
     <row r="26">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>829.45</v>
+        <v>812.5</v>
       </c>
       <c r="C26" s="12" t="n">
-        <v>811</v>
+        <v>794.9</v>
       </c>
       <c r="D26" s="15" t="n">
-        <v>822.5</v>
+        <v>798.5</v>
       </c>
       <c r="E26" s="6" t="n">
-        <v>821.9</v>
+        <v>796.4</v>
       </c>
       <c r="F26" s="18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G26" s="6" t="n">
-        <v>813.45</v>
+        <v>807.1</v>
       </c>
     </row>
     <row r="27">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>1096</v>
+        <v>1088.25</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>1081.5</v>
+        <v>1076.3</v>
       </c>
       <c r="D27" s="15" t="n">
-        <v>1082.1</v>
+        <v>1081.45</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>1082.65</v>
+        <v>1081.25</v>
       </c>
       <c r="F27" s="18" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>1083.8</v>
+        <v>1079.3</v>
       </c>
     </row>
     <row r="28">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>1115</v>
+        <v>1084</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>1097.45</v>
+        <v>1066.95</v>
       </c>
       <c r="D28" s="15" t="n">
-        <v>1109</v>
+        <v>1068.7</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>1111.35</v>
+        <v>1069.15</v>
       </c>
       <c r="F28" s="18" t="n">
-        <v>176</v>
+        <v>79</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>1111.5</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="29">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B29" s="9" t="n">
-        <v>437.4</v>
+        <v>424</v>
       </c>
       <c r="C29" s="12" t="n">
-        <v>431.8</v>
+        <v>419.15</v>
       </c>
       <c r="D29" s="15" t="n">
-        <v>434.95</v>
+        <v>420.7</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>434.65</v>
+        <v>420.9</v>
       </c>
       <c r="F29" s="18" t="n">
-        <v>128</v>
+        <v>81</v>
       </c>
       <c r="G29" s="6" t="n">
-        <v>432.25</v>
+        <v>421.3</v>
       </c>
     </row>
     <row r="30">
@@ -1347,22 +1347,22 @@
         </is>
       </c>
       <c r="B30" s="9" t="n">
-        <v>155.25</v>
+        <v>152.79</v>
       </c>
       <c r="C30" s="12" t="n">
-        <v>152.47</v>
+        <v>151.4</v>
       </c>
       <c r="D30" s="15" t="n">
-        <v>153.3</v>
+        <v>152.03</v>
       </c>
       <c r="E30" s="6" t="n">
-        <v>152.76</v>
+        <v>151.72</v>
       </c>
       <c r="F30" s="18" t="n">
-        <v>551</v>
+        <v>283</v>
       </c>
       <c r="G30" s="6" t="n">
-        <v>153.62</v>
+        <v>152.66</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" thickBot="1">
@@ -1372,22 +1372,22 @@
         </is>
       </c>
       <c r="B31" s="10" t="n">
-        <v>11360.9</v>
+        <v>11822.75</v>
       </c>
       <c r="C31" s="13" t="n">
-        <v>11255</v>
+        <v>11514.2</v>
       </c>
       <c r="D31" s="16" t="n">
-        <v>11320</v>
+        <v>11532</v>
       </c>
       <c r="E31" s="7" t="n">
-        <v>11301.9</v>
+        <v>11542.65</v>
       </c>
       <c r="F31" s="19" t="n">
         <v>4</v>
       </c>
       <c r="G31" s="7" t="n">
-        <v>11278.7</v>
+        <v>11781.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed 6 jun 24 error in algo shares
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -597,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>593.85</v>
+        <v>592.8</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>581.7</v>
+        <v>581.3</v>
       </c>
       <c r="D2" s="14" t="n">
-        <v>583.65</v>
+        <v>588</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>583.4</v>
+        <v>587</v>
       </c>
       <c r="F2" s="17" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>586.8</v>
+        <v>583.2</v>
       </c>
     </row>
     <row r="3">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>3179</v>
+        <v>3192</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>3116</v>
+        <v>3107</v>
       </c>
       <c r="D3" s="14" t="n">
-        <v>3137.65</v>
+        <v>3183</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>3130.3</v>
+        <v>3186.1</v>
       </c>
       <c r="F3" s="17" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>3127</v>
+        <v>3131.2</v>
       </c>
     </row>
     <row r="4">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>555.9</v>
+        <v>552.15</v>
       </c>
       <c r="C4" s="12" t="n">
-        <v>545</v>
+        <v>546.2</v>
       </c>
       <c r="D4" s="15" t="n">
         <v>547.1</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>547.55</v>
+        <v>550.75</v>
       </c>
       <c r="F4" s="18" t="n">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>551.25</v>
+        <v>549.6</v>
       </c>
     </row>
     <row r="5">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>2029.9</v>
+        <v>2007.1</v>
       </c>
       <c r="C5" s="12" t="n">
-        <v>1971.2</v>
+        <v>1970.4</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>2004.75</v>
+        <v>1975.2</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>2010.7</v>
+        <v>1975.25</v>
       </c>
       <c r="F5" s="18" t="n">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>1973</v>
+        <v>1979.6</v>
       </c>
     </row>
     <row r="6">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>7810</v>
+        <v>7814.65</v>
       </c>
       <c r="C6" s="12" t="n">
-        <v>7712</v>
+        <v>7656.25</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>7748</v>
+        <v>7722</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>7756</v>
+        <v>7703</v>
       </c>
       <c r="F6" s="18" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>7714.5</v>
+        <v>7670.7</v>
       </c>
     </row>
     <row r="7">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>206.9</v>
+        <v>198.03</v>
       </c>
       <c r="C7" s="12" t="n">
-        <v>202.3</v>
+        <v>195</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>203.93</v>
+        <v>195.48</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>203.22</v>
+        <v>195.28</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>268</v>
+        <v>134</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>206.25</v>
+        <v>197.72</v>
       </c>
     </row>
     <row r="8">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>250</v>
+        <v>251.4</v>
       </c>
       <c r="C8" s="12" t="n">
-        <v>244.95</v>
+        <v>248.1</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>248.1</v>
+        <v>248.3</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>249.6</v>
+        <v>248.91</v>
       </c>
       <c r="F8" s="18" t="n">
-        <v>215</v>
+        <v>87</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>244.95</v>
+        <v>250.75</v>
       </c>
     </row>
     <row r="9">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>517.85</v>
+        <v>516</v>
       </c>
       <c r="C9" s="12" t="n">
-        <v>506.2</v>
+        <v>506.15</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>513</v>
+        <v>508.5</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>516.1</v>
+        <v>508.5</v>
       </c>
       <c r="F9" s="18" t="n">
-        <v>154</v>
+        <v>47</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>506.3</v>
+        <v>515.8</v>
       </c>
     </row>
     <row r="10">
@@ -847,22 +847,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>929</v>
+        <v>916.1</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>905</v>
+        <v>895.3</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>915</v>
+        <v>912.55</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>914.05</v>
+        <v>913.75</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>926.15</v>
+        <v>904.75</v>
       </c>
     </row>
     <row r="11">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>5105</v>
+        <v>5016.35</v>
       </c>
       <c r="C11" s="12" t="n">
-        <v>4976</v>
+        <v>4952</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>5062.75</v>
+        <v>4977.4</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>5062.6</v>
+        <v>4972.65</v>
       </c>
       <c r="F11" s="18" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>5012.75</v>
+        <v>5013.3</v>
       </c>
     </row>
     <row r="12">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>195.5</v>
+        <v>200.1</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>191.01</v>
+        <v>196.27</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>193.25</v>
+        <v>197.3</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>193.71</v>
+        <v>197.12</v>
       </c>
       <c r="F12" s="18" t="n">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>191.12</v>
+        <v>196.71</v>
       </c>
     </row>
     <row r="13">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>1828.55</v>
+        <v>1822.45</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>1796.55</v>
+        <v>1794.6</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>1809</v>
+        <v>1816.45</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>1808.4</v>
+        <v>1816.5</v>
       </c>
       <c r="F13" s="18" t="n">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>1826</v>
+        <v>1802.75</v>
       </c>
     </row>
     <row r="14">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>1775.8</v>
+        <v>1740.5</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>1750</v>
+        <v>1720.1</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>1753</v>
+        <v>1728.3</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>1752.65</v>
+        <v>1726.2</v>
       </c>
       <c r="F14" s="18" t="n">
-        <v>178</v>
+        <v>122</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>1770.15</v>
+        <v>1739.6</v>
       </c>
     </row>
     <row r="15">
@@ -972,22 +972,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>757.7</v>
+        <v>765.5</v>
       </c>
       <c r="C15" s="12" t="n">
-        <v>744.65</v>
+        <v>745.2</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>744.65</v>
+        <v>760</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>747.15</v>
+        <v>761.55</v>
       </c>
       <c r="F15" s="18" t="n">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>750.4</v>
+        <v>752.05</v>
       </c>
     </row>
     <row r="16">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1326.25</v>
+        <v>1280.25</v>
       </c>
       <c r="C16" s="12" t="n">
-        <v>1303.85</v>
+        <v>1267.6</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>1306.5</v>
+        <v>1277</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1306.6</v>
+        <v>1274.4</v>
       </c>
       <c r="F16" s="18" t="n">
-        <v>171</v>
+        <v>109</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1323.7</v>
+        <v>1279.15</v>
       </c>
     </row>
     <row r="17">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1481</v>
+        <v>1449.05</v>
       </c>
       <c r="C17" s="12" t="n">
-        <v>1459.2</v>
+        <v>1404.65</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>1462</v>
+        <v>1409.15</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1462.7</v>
+        <v>1409.7</v>
       </c>
       <c r="F17" s="18" t="n">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1464.25</v>
+        <v>1444.95</v>
       </c>
     </row>
     <row r="18">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>1974.6</v>
+        <v>1908.95</v>
       </c>
       <c r="C18" s="12" t="n">
-        <v>1903.3</v>
+        <v>1883.1</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>1906.75</v>
+        <v>1904.35</v>
       </c>
       <c r="F18" s="18" t="n">
-        <v>149</v>
+        <v>40</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>1967.15</v>
+        <v>1890.25</v>
       </c>
     </row>
     <row r="19">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>1044.05</v>
+        <v>1039.6</v>
       </c>
       <c r="C19" s="12" t="n">
-        <v>1011.1</v>
+        <v>1019.45</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>1020.45</v>
+        <v>1033.45</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>1028.05</v>
+        <v>1035.35</v>
       </c>
       <c r="F19" s="18" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>1035.15</v>
+        <v>1038.65</v>
       </c>
     </row>
     <row r="20">
@@ -1097,22 +1097,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>671.35</v>
+        <v>668.75</v>
       </c>
       <c r="C20" s="12" t="n">
-        <v>663.05</v>
+        <v>657.5</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>665</v>
+        <v>658.5</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>664</v>
+        <v>659.25</v>
       </c>
       <c r="F20" s="18" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>666.3</v>
+        <v>666</v>
       </c>
     </row>
     <row r="21">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>3222.1</v>
+        <v>3185.45</v>
       </c>
       <c r="C21" s="12" t="n">
-        <v>3152.55</v>
+        <v>3111.55</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>3190</v>
+        <v>3168</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>3183.65</v>
+        <v>3165.5</v>
       </c>
       <c r="F21" s="18" t="n">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>3160.35</v>
+        <v>3128.7</v>
       </c>
     </row>
     <row r="22">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>343</v>
+        <v>338.45</v>
       </c>
       <c r="C22" s="12" t="n">
-        <v>332.1</v>
+        <v>328.05</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>334.95</v>
+        <v>332.55</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>333.5</v>
+        <v>330.1</v>
       </c>
       <c r="F22" s="18" t="n">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>339</v>
+        <v>337.75</v>
       </c>
     </row>
     <row r="23">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>442.5</v>
+        <v>446.55</v>
       </c>
       <c r="C23" s="12" t="n">
-        <v>434.05</v>
+        <v>438.8</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>440.3</v>
+        <v>440.8</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>436.9</v>
+        <v>440.1</v>
       </c>
       <c r="F23" s="18" t="n">
-        <v>538</v>
+        <v>159</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>435.2</v>
+        <v>444.6</v>
       </c>
     </row>
     <row r="24">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>3066.95</v>
+        <v>2967.65</v>
       </c>
       <c r="C24" s="12" t="n">
-        <v>2984</v>
+        <v>2925.65</v>
       </c>
       <c r="D24" s="15" t="n">
-        <v>3047.05</v>
+        <v>2927</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>3052.35</v>
+        <v>2929.65</v>
       </c>
       <c r="F24" s="18" t="n">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>2994.1</v>
+        <v>2967.35</v>
       </c>
     </row>
     <row r="25">
@@ -1222,22 +1222,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>808</v>
+        <v>800.35</v>
       </c>
       <c r="C25" s="12" t="n">
-        <v>798.45</v>
+        <v>791.7</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>802.3</v>
+        <v>795.5</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>802.65</v>
+        <v>796.95</v>
       </c>
       <c r="F25" s="18" t="n">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>803.4</v>
+        <v>794.75</v>
       </c>
     </row>
     <row r="26">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>853.7</v>
+        <v>853</v>
       </c>
       <c r="C26" s="12" t="n">
-        <v>832</v>
+        <v>833.85</v>
       </c>
       <c r="D26" s="15" t="n">
+        <v>849.3</v>
+      </c>
+      <c r="E26" s="6" t="n">
+        <v>849.65</v>
+      </c>
+      <c r="F26" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="G26" s="6" t="n">
         <v>837.5</v>
-      </c>
-      <c r="E26" s="6" t="n">
-        <v>835.05</v>
-      </c>
-      <c r="F26" s="18" t="n">
-        <v>7</v>
-      </c>
-      <c r="G26" s="6" t="n">
-        <v>834.3</v>
       </c>
     </row>
     <row r="27">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>1089.8</v>
+        <v>1139.95</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>1064.1</v>
+        <v>1090.35</v>
       </c>
       <c r="D27" s="15" t="n">
-        <v>1066.45</v>
+        <v>1130.9</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>1067.2</v>
+        <v>1132.6</v>
       </c>
       <c r="F27" s="18" t="n">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>1067.75</v>
+        <v>1093.8</v>
       </c>
     </row>
     <row r="28">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>998.7</v>
+        <v>984.5</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>989.15</v>
+        <v>958.9</v>
       </c>
       <c r="D28" s="15" t="n">
-        <v>989.9</v>
+        <v>966.4</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>993</v>
+        <v>965.2</v>
       </c>
       <c r="F28" s="18" t="n">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>991.15</v>
+        <v>980</v>
       </c>
     </row>
     <row r="29">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B29" s="9" t="n">
-        <v>494.85</v>
+        <v>491.2</v>
       </c>
       <c r="C29" s="12" t="n">
-        <v>477.5</v>
+        <v>479.4</v>
       </c>
       <c r="D29" s="15" t="n">
-        <v>484.4</v>
+        <v>481</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>485.5</v>
+        <v>481.25</v>
       </c>
       <c r="F29" s="18" t="n">
-        <v>321</v>
+        <v>151</v>
       </c>
       <c r="G29" s="6" t="n">
-        <v>480.5</v>
+        <v>486.7</v>
       </c>
     </row>
     <row r="30">
@@ -1347,22 +1347,22 @@
         </is>
       </c>
       <c r="B30" s="9" t="n">
-        <v>169.01</v>
+        <v>168.37</v>
       </c>
       <c r="C30" s="12" t="n">
-        <v>165.89</v>
+        <v>165.1</v>
       </c>
       <c r="D30" s="15" t="n">
-        <v>166.13</v>
+        <v>166.7</v>
       </c>
       <c r="E30" s="6" t="n">
-        <v>166.55</v>
+        <v>167.03</v>
       </c>
       <c r="F30" s="18" t="n">
-        <v>727</v>
+        <v>507</v>
       </c>
       <c r="G30" s="6" t="n">
-        <v>167</v>
+        <v>168.12</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" thickBot="1">
@@ -1372,22 +1372,22 @@
         </is>
       </c>
       <c r="B31" s="10" t="n">
-        <v>12138</v>
+        <v>11887.7</v>
       </c>
       <c r="C31" s="13" t="n">
-        <v>11924.75</v>
+        <v>11650.25</v>
       </c>
       <c r="D31" s="16" t="n">
-        <v>11950</v>
+        <v>11849.85</v>
       </c>
       <c r="E31" s="7" t="n">
-        <v>11952.3</v>
+        <v>11837.15</v>
       </c>
       <c r="F31" s="19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G31" s="7" t="n">
-        <v>12062.05</v>
+        <v>11798.8</v>
       </c>
     </row>
   </sheetData>
@@ -1402,10 +1402,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:G29"/>
+      <selection activeCell="L9" sqref="L9:O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1546,6 +1546,24 @@
       <c r="E9" s="1" t="n"/>
       <c r="F9" s="1" t="n"/>
       <c r="G9" s="1" t="n"/>
+      <c r="J9" t="n">
+        <v>587.5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>579.1</v>
+      </c>
+      <c r="L9" t="n">
+        <v>582.15</v>
+      </c>
+      <c r="M9" t="n">
+        <v>582.95</v>
+      </c>
+      <c r="N9" t="n">
+        <v>10</v>
+      </c>
+      <c r="O9" t="n">
+        <v>586</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1559,6 +1577,24 @@
       <c r="E10" s="1" t="n"/>
       <c r="F10" s="1" t="n"/>
       <c r="G10" s="1" t="n"/>
+      <c r="J10" t="n">
+        <v>3179</v>
+      </c>
+      <c r="K10" t="n">
+        <v>3116</v>
+      </c>
+      <c r="L10" t="n">
+        <v>3131</v>
+      </c>
+      <c r="M10" t="n">
+        <v>3135.85</v>
+      </c>
+      <c r="N10" t="n">
+        <v>16</v>
+      </c>
+      <c r="O10" t="n">
+        <v>3127</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1572,6 +1608,24 @@
       <c r="E11" s="1" t="n"/>
       <c r="F11" s="1" t="n"/>
       <c r="G11" s="1" t="n"/>
+      <c r="J11" t="n">
+        <v>555.9</v>
+      </c>
+      <c r="K11" t="n">
+        <v>545</v>
+      </c>
+      <c r="L11" t="n">
+        <v>547.9</v>
+      </c>
+      <c r="M11" t="n">
+        <v>547.85</v>
+      </c>
+      <c r="N11" t="n">
+        <v>13</v>
+      </c>
+      <c r="O11" t="n">
+        <v>551.25</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1585,6 +1639,24 @@
       <c r="E12" s="1" t="n"/>
       <c r="F12" s="1" t="n"/>
       <c r="G12" s="1" t="n"/>
+      <c r="J12" t="n">
+        <v>2029.9</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1971.2</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1969.65</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1973.4</v>
+      </c>
+      <c r="N12" t="n">
+        <v>18</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1973</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1598,6 +1670,24 @@
       <c r="E13" s="1" t="n"/>
       <c r="F13" s="1" t="n"/>
       <c r="G13" s="1" t="n"/>
+      <c r="J13" t="n">
+        <v>7810</v>
+      </c>
+      <c r="K13" t="n">
+        <v>7712</v>
+      </c>
+      <c r="L13" t="n">
+        <v>7697.85</v>
+      </c>
+      <c r="M13" t="n">
+        <v>7703</v>
+      </c>
+      <c r="N13" t="n">
+        <v>9</v>
+      </c>
+      <c r="O13" t="n">
+        <v>7714.5</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1611,6 +1701,24 @@
       <c r="E14" s="1" t="n"/>
       <c r="F14" s="1" t="n"/>
       <c r="G14" s="1" t="n"/>
+      <c r="J14" t="n">
+        <v>3209.9</v>
+      </c>
+      <c r="K14" t="n">
+        <v>3120.6</v>
+      </c>
+      <c r="L14" t="n">
+        <v>198.45</v>
+      </c>
+      <c r="M14" t="n">
+        <v>198.74</v>
+      </c>
+      <c r="N14" t="n">
+        <v>94</v>
+      </c>
+      <c r="O14" t="n">
+        <v>3143</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1624,6 +1732,24 @@
       <c r="E15" s="1" t="n"/>
       <c r="F15" s="1" t="n"/>
       <c r="G15" s="1" t="n"/>
+      <c r="J15" t="n">
+        <v>551</v>
+      </c>
+      <c r="K15" t="n">
+        <v>538.5</v>
+      </c>
+      <c r="L15" t="n">
+        <v>247</v>
+      </c>
+      <c r="M15" t="n">
+        <v>247.8</v>
+      </c>
+      <c r="N15" t="n">
+        <v>129</v>
+      </c>
+      <c r="O15" t="n">
+        <v>543.8</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1637,6 +1763,24 @@
       <c r="E16" s="1" t="n"/>
       <c r="F16" s="1" t="n"/>
       <c r="G16" s="1" t="n"/>
+      <c r="J16" t="n">
+        <v>2018.95</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1968.3</v>
+      </c>
+      <c r="L16" t="n">
+        <v>509.4</v>
+      </c>
+      <c r="M16" t="n">
+        <v>510.15</v>
+      </c>
+      <c r="N16" t="n">
+        <v>88</v>
+      </c>
+      <c r="O16" t="n">
+        <v>2008.3</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1650,6 +1794,24 @@
       <c r="E17" s="1" t="n"/>
       <c r="F17" s="1" t="n"/>
       <c r="G17" s="1" t="n"/>
+      <c r="J17" t="n">
+        <v>7800</v>
+      </c>
+      <c r="K17" t="n">
+        <v>7676.15</v>
+      </c>
+      <c r="L17" t="n">
+        <v>895.45</v>
+      </c>
+      <c r="M17" t="n">
+        <v>895.15</v>
+      </c>
+      <c r="N17" t="n">
+        <v>46</v>
+      </c>
+      <c r="O17" t="n">
+        <v>7757.75</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1663,6 +1825,24 @@
       <c r="E18" s="1" t="n"/>
       <c r="F18" s="1" t="n"/>
       <c r="G18" s="1" t="n"/>
+      <c r="J18" t="n">
+        <v>204.3</v>
+      </c>
+      <c r="K18" t="n">
+        <v>197.85</v>
+      </c>
+      <c r="L18" t="n">
+        <v>5036.15</v>
+      </c>
+      <c r="M18" t="n">
+        <v>5026.25</v>
+      </c>
+      <c r="N18" t="n">
+        <v>5</v>
+      </c>
+      <c r="O18" t="n">
+        <v>203.81</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -1676,6 +1856,24 @@
       <c r="E19" s="1" t="n"/>
       <c r="F19" s="1" t="n"/>
       <c r="G19" s="1" t="n"/>
+      <c r="J19" t="n">
+        <v>251.6</v>
+      </c>
+      <c r="K19" t="n">
+        <v>246.15</v>
+      </c>
+      <c r="L19" t="n">
+        <v>196.69</v>
+      </c>
+      <c r="M19" t="n">
+        <v>196.73</v>
+      </c>
+      <c r="N19" t="n">
+        <v>129</v>
+      </c>
+      <c r="O19" t="n">
+        <v>248.6</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1689,6 +1887,24 @@
       <c r="E20" s="1" t="n"/>
       <c r="F20" s="1" t="n"/>
       <c r="G20" s="1" t="n"/>
+      <c r="J20" t="n">
+        <v>513.45</v>
+      </c>
+      <c r="K20" t="n">
+        <v>502.5</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1796</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1796.1</v>
+      </c>
+      <c r="N20" t="n">
+        <v>21</v>
+      </c>
+      <c r="O20" t="n">
+        <v>508.25</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1702,6 +1918,24 @@
       <c r="E21" s="1" t="n"/>
       <c r="F21" s="1" t="n"/>
       <c r="G21" s="1" t="n"/>
+      <c r="J21" t="n">
+        <v>916.35</v>
+      </c>
+      <c r="K21" t="n">
+        <v>893.05</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1732</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1732.05</v>
+      </c>
+      <c r="N21" t="n">
+        <v>131</v>
+      </c>
+      <c r="O21" t="n">
+        <v>916.3</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -1715,6 +1949,24 @@
       <c r="E22" s="1" t="n"/>
       <c r="F22" s="1" t="n"/>
       <c r="G22" s="1" t="n"/>
+      <c r="J22" t="n">
+        <v>5085</v>
+      </c>
+      <c r="K22" t="n">
+        <v>4998.5</v>
+      </c>
+      <c r="L22" t="n">
+        <v>755</v>
+      </c>
+      <c r="M22" t="n">
+        <v>756.2</v>
+      </c>
+      <c r="N22" t="n">
+        <v>85</v>
+      </c>
+      <c r="O22" t="n">
+        <v>5050</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1728,6 +1980,24 @@
       <c r="E23" s="1" t="n"/>
       <c r="F23" s="1" t="n"/>
       <c r="G23" s="1" t="n"/>
+      <c r="J23" t="n">
+        <v>197.7</v>
+      </c>
+      <c r="K23" t="n">
+        <v>192.9</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1273.95</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1273</v>
+      </c>
+      <c r="N23" t="n">
+        <v>126</v>
+      </c>
+      <c r="O23" t="n">
+        <v>194.92</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -1741,6 +2011,24 @@
       <c r="E24" s="1" t="n"/>
       <c r="F24" s="1" t="n"/>
       <c r="G24" s="1" t="n"/>
+      <c r="J24" t="n">
+        <v>1820.7</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1789.15</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1445</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1447.6</v>
+      </c>
+      <c r="N24" t="n">
+        <v>28</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1810.4</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -1754,6 +2042,24 @@
       <c r="E25" s="1" t="n"/>
       <c r="F25" s="1" t="n"/>
       <c r="G25" s="1" t="n"/>
+      <c r="J25" t="n">
+        <v>1750.75</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1724.4</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1877.6</v>
+      </c>
+      <c r="M25" t="n">
+        <v>1875.6</v>
+      </c>
+      <c r="N25" t="n">
+        <v>69</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1748.95</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -1767,6 +2073,24 @@
       <c r="E26" s="1" t="n"/>
       <c r="F26" s="1" t="n"/>
       <c r="G26" s="1" t="n"/>
+      <c r="J26" t="n">
+        <v>763.2</v>
+      </c>
+      <c r="K26" t="n">
+        <v>753.15</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1038</v>
+      </c>
+      <c r="M26" t="n">
+        <v>1039.65</v>
+      </c>
+      <c r="N26" t="n">
+        <v>30</v>
+      </c>
+      <c r="O26" t="n">
+        <v>760.65</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -1780,6 +2104,24 @@
       <c r="E27" s="1" t="n"/>
       <c r="F27" s="1" t="n"/>
       <c r="G27" s="1" t="n"/>
+      <c r="J27" t="n">
+        <v>1291.7</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1270.9</v>
+      </c>
+      <c r="L27" t="n">
+        <v>662.9</v>
+      </c>
+      <c r="M27" t="n">
+        <v>662.45</v>
+      </c>
+      <c r="N27" t="n">
+        <v>12</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1289.2</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -1793,6 +2135,24 @@
       <c r="E28" s="1" t="n"/>
       <c r="F28" s="1" t="n"/>
       <c r="G28" s="1" t="n"/>
+      <c r="J28" t="n">
+        <v>1455.9</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1437</v>
+      </c>
+      <c r="L28" t="n">
+        <v>3115</v>
+      </c>
+      <c r="M28" t="n">
+        <v>3094.9</v>
+      </c>
+      <c r="N28" t="n">
+        <v>35</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1455</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -1806,6 +2166,204 @@
       <c r="E29" s="1" t="n"/>
       <c r="F29" s="1" t="n"/>
       <c r="G29" s="1" t="n"/>
+      <c r="J29" t="n">
+        <v>1901.25</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1870.5</v>
+      </c>
+      <c r="L29" t="n">
+        <v>340.35</v>
+      </c>
+      <c r="M29" t="n">
+        <v>338.35</v>
+      </c>
+      <c r="N29" t="n">
+        <v>49</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1889.55</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="J30" t="n">
+        <v>1058.85</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1023.55</v>
+      </c>
+      <c r="L30" t="n">
+        <v>443</v>
+      </c>
+      <c r="M30" t="n">
+        <v>443.2</v>
+      </c>
+      <c r="N30" t="n">
+        <v>209</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1032.45</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="J31" t="n">
+        <v>670.55</v>
+      </c>
+      <c r="K31" t="n">
+        <v>659.25</v>
+      </c>
+      <c r="L31" t="n">
+        <v>2958</v>
+      </c>
+      <c r="M31" t="n">
+        <v>2953.15</v>
+      </c>
+      <c r="N31" t="n">
+        <v>135</v>
+      </c>
+      <c r="O31" t="n">
+        <v>662.8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="J32" t="n">
+        <v>3151.95</v>
+      </c>
+      <c r="K32" t="n">
+        <v>3087</v>
+      </c>
+      <c r="L32" t="n">
+        <v>788</v>
+      </c>
+      <c r="M32" t="n">
+        <v>787.9</v>
+      </c>
+      <c r="N32" t="n">
+        <v>154</v>
+      </c>
+      <c r="O32" t="n">
+        <v>3137.2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="J33" t="n">
+        <v>341.65</v>
+      </c>
+      <c r="K33" t="n">
+        <v>330.65</v>
+      </c>
+      <c r="L33" t="n">
+        <v>833.5</v>
+      </c>
+      <c r="M33" t="n">
+        <v>833.1</v>
+      </c>
+      <c r="N33" t="n">
+        <v>2</v>
+      </c>
+      <c r="O33" t="n">
+        <v>334.75</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="J34" t="n">
+        <v>445.95</v>
+      </c>
+      <c r="K34" t="n">
+        <v>433.6</v>
+      </c>
+      <c r="L34" t="n">
+        <v>1091.5</v>
+      </c>
+      <c r="M34" t="n">
+        <v>1091.1</v>
+      </c>
+      <c r="N34" t="n">
+        <v>24</v>
+      </c>
+      <c r="O34" t="n">
+        <v>444.4</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="J35" t="n">
+        <v>3027.5</v>
+      </c>
+      <c r="K35" t="n">
+        <v>2948.8</v>
+      </c>
+      <c r="L35" t="n">
+        <v>975.8</v>
+      </c>
+      <c r="M35" t="n">
+        <v>974.65</v>
+      </c>
+      <c r="N35" t="n">
+        <v>122</v>
+      </c>
+      <c r="O35" t="n">
+        <v>3025.35</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="J36" t="n">
+        <v>799.3</v>
+      </c>
+      <c r="K36" t="n">
+        <v>786.45</v>
+      </c>
+      <c r="L36" t="n">
+        <v>482.5</v>
+      </c>
+      <c r="M36" t="n">
+        <v>482.6</v>
+      </c>
+      <c r="N36" t="n">
+        <v>157</v>
+      </c>
+      <c r="O36" t="n">
+        <v>798.8</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="J37" t="n">
+        <v>837.95</v>
+      </c>
+      <c r="K37" t="n">
+        <v>824.4</v>
+      </c>
+      <c r="L37" t="n">
+        <v>168.11</v>
+      </c>
+      <c r="M37" t="n">
+        <v>168.55</v>
+      </c>
+      <c r="N37" t="n">
+        <v>923</v>
+      </c>
+      <c r="O37" t="n">
+        <v>832.95</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="J38" t="n">
+        <v>1101.3</v>
+      </c>
+      <c r="K38" t="n">
+        <v>1074.15</v>
+      </c>
+      <c r="L38" t="n">
+        <v>11800</v>
+      </c>
+      <c r="M38" t="n">
+        <v>11802</v>
+      </c>
+      <c r="N38" t="n">
+        <v>4</v>
+      </c>
+      <c r="O38" t="n">
+        <v>1092.15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
moved algo folder and will only keep new algo shares in algo folder, all shares (new + old) get put in algo old
</commit_message>
<xml_diff>
--- a/cash high low.xlsx
+++ b/cash high low.xlsx
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>592.8</v>
+        <v>531.9</v>
       </c>
       <c r="C2" s="11" t="n">
-        <v>581.3</v>
+        <v>526</v>
       </c>
       <c r="D2" s="14" t="n">
-        <v>588</v>
+        <v>530.05</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>587</v>
+        <v>529.2</v>
       </c>
       <c r="F2" s="17" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>583.2</v>
+        <v>528.35</v>
       </c>
     </row>
     <row r="3">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>3192</v>
+        <v>3190</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>3107</v>
+        <v>3116</v>
       </c>
       <c r="D3" s="14" t="n">
-        <v>3183</v>
+        <v>3129.95</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>3186.1</v>
+        <v>3137.2</v>
       </c>
       <c r="F3" s="17" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>3131.2</v>
+        <v>3186.8</v>
       </c>
     </row>
     <row r="4">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>552.15</v>
+        <v>510.95</v>
       </c>
       <c r="C4" s="12" t="n">
-        <v>546.2</v>
+        <v>501.25</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>547.1</v>
+        <v>504.7</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>550.75</v>
+        <v>505.05</v>
       </c>
       <c r="F4" s="18" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G4" s="6" t="n">
-        <v>549.6</v>
+        <v>505.6</v>
       </c>
     </row>
     <row r="5">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>2007.1</v>
+        <v>1879.9</v>
       </c>
       <c r="C5" s="12" t="n">
-        <v>1970.4</v>
+        <v>1855.1</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>1975.2</v>
+        <v>1877.95</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>1975.25</v>
+        <v>1876.4</v>
       </c>
       <c r="F5" s="18" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>1979.6</v>
+        <v>1864.3</v>
       </c>
     </row>
     <row r="6">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B6" s="9" t="n">
-        <v>7814.65</v>
+        <v>7317.95</v>
       </c>
       <c r="C6" s="12" t="n">
-        <v>7656.25</v>
+        <v>7226.05</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>7722</v>
+        <v>7300.1</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>7703</v>
+        <v>7302</v>
       </c>
       <c r="F6" s="18" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G6" s="6" t="n">
-        <v>7670.7</v>
+        <v>7262.7</v>
       </c>
     </row>
     <row r="7">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B7" s="9" t="n">
-        <v>198.03</v>
+        <v>211.8</v>
       </c>
       <c r="C7" s="12" t="n">
-        <v>195</v>
+        <v>200.25</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>195.48</v>
+        <v>209.44</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>195.28</v>
+        <v>210.26</v>
       </c>
       <c r="F7" s="18" t="n">
-        <v>134</v>
+        <v>1298</v>
       </c>
       <c r="G7" s="6" t="n">
-        <v>197.72</v>
+        <v>201.35</v>
       </c>
     </row>
     <row r="8">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>251.4</v>
+        <v>248.2</v>
       </c>
       <c r="C8" s="12" t="n">
-        <v>248.1</v>
+        <v>242.13</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>248.3</v>
+        <v>242.48</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>248.91</v>
+        <v>242.42</v>
       </c>
       <c r="F8" s="18" t="n">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>250.75</v>
+        <v>246.75</v>
       </c>
     </row>
     <row r="9">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>516</v>
+        <v>493.9</v>
       </c>
       <c r="C9" s="12" t="n">
-        <v>506.15</v>
+        <v>488</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>508.5</v>
+        <v>493.1</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>508.5</v>
+        <v>492.95</v>
       </c>
       <c r="F9" s="18" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G9" s="6" t="n">
-        <v>515.8</v>
+        <v>488.6</v>
       </c>
     </row>
     <row r="10">
@@ -847,22 +847,22 @@
         </is>
       </c>
       <c r="B10" s="9" t="n">
-        <v>916.1</v>
+        <v>859.75</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>895.3</v>
+        <v>841.75</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>912.55</v>
+        <v>845.8</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>913.75</v>
+        <v>846.6</v>
       </c>
       <c r="F10" s="18" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G10" s="6" t="n">
-        <v>904.75</v>
+        <v>854.35</v>
       </c>
     </row>
     <row r="11">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>5016.35</v>
+        <v>4808.15</v>
       </c>
       <c r="C11" s="12" t="n">
-        <v>4952</v>
+        <v>4664.15</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>4977.4</v>
+        <v>4735.9</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>4972.65</v>
+        <v>4728.05</v>
       </c>
       <c r="F11" s="18" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G11" s="6" t="n">
-        <v>5013.3</v>
+        <v>4670.05</v>
       </c>
     </row>
     <row r="12">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>200.1</v>
+        <v>189.3</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>196.27</v>
+        <v>186.63</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>197.3</v>
+        <v>187.58</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>197.12</v>
+        <v>187.55</v>
       </c>
       <c r="F12" s="18" t="n">
-        <v>162</v>
+        <v>52</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>196.71</v>
+        <v>187.15</v>
       </c>
     </row>
     <row r="13">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>1822.45</v>
+        <v>1852.8</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>1794.6</v>
+        <v>1821</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>1816.45</v>
+        <v>1839.95</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>1816.5</v>
+        <v>1839.65</v>
       </c>
       <c r="F13" s="18" t="n">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="G13" s="6" t="n">
-        <v>1802.75</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="14">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>1740.5</v>
+        <v>1659.05</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>1720.1</v>
+        <v>1643.25</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>1728.3</v>
+        <v>1651.5</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>1726.2</v>
+        <v>1651</v>
       </c>
       <c r="F14" s="18" t="n">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G14" s="6" t="n">
-        <v>1739.6</v>
+        <v>1652.15</v>
       </c>
     </row>
     <row r="15">
@@ -972,22 +972,22 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>765.5</v>
+        <v>749.95</v>
       </c>
       <c r="C15" s="12" t="n">
-        <v>745.2</v>
+        <v>736.05</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>760</v>
+        <v>746.7</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>761.55</v>
+        <v>747.35</v>
       </c>
       <c r="F15" s="18" t="n">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G15" s="6" t="n">
-        <v>752.05</v>
+        <v>737.6</v>
       </c>
     </row>
     <row r="16">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B16" s="9" t="n">
-        <v>1280.25</v>
+        <v>1237.55</v>
       </c>
       <c r="C16" s="12" t="n">
-        <v>1267.6</v>
+        <v>1222</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>1277</v>
+        <v>1223.3</v>
       </c>
       <c r="E16" s="6" t="n">
-        <v>1274.4</v>
+        <v>1223</v>
       </c>
       <c r="F16" s="18" t="n">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="G16" s="6" t="n">
-        <v>1279.15</v>
+        <v>1234.7</v>
       </c>
     </row>
     <row r="17">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B17" s="9" t="n">
-        <v>1449.05</v>
+        <v>1371.3</v>
       </c>
       <c r="C17" s="12" t="n">
-        <v>1404.65</v>
+        <v>1339</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>1409.15</v>
+        <v>1347.85</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>1409.7</v>
+        <v>1347.6</v>
       </c>
       <c r="F17" s="18" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G17" s="6" t="n">
-        <v>1444.95</v>
+        <v>1356.15</v>
       </c>
     </row>
     <row r="18">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>1908.95</v>
+        <v>1947</v>
       </c>
       <c r="C18" s="12" t="n">
-        <v>1883.1</v>
+        <v>1915.5</v>
       </c>
       <c r="D18" s="15" t="n">
-        <v>1906</v>
+        <v>1935</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>1904.35</v>
+        <v>1935.1</v>
       </c>
       <c r="F18" s="18" t="n">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G18" s="6" t="n">
-        <v>1890.25</v>
+        <v>1920.65</v>
       </c>
     </row>
     <row r="19">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B19" s="9" t="n">
-        <v>1039.6</v>
+        <v>1014</v>
       </c>
       <c r="C19" s="12" t="n">
-        <v>1019.45</v>
+        <v>996.65</v>
       </c>
       <c r="D19" s="15" t="n">
-        <v>1033.45</v>
+        <v>1003.9</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>1035.35</v>
+        <v>1005.85</v>
       </c>
       <c r="F19" s="18" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G19" s="6" t="n">
-        <v>1038.65</v>
+        <v>997.45</v>
       </c>
     </row>
     <row r="20">
@@ -1097,22 +1097,22 @@
         </is>
       </c>
       <c r="B20" s="9" t="n">
-        <v>668.75</v>
+        <v>621.65</v>
       </c>
       <c r="C20" s="12" t="n">
-        <v>657.5</v>
+        <v>614.15</v>
       </c>
       <c r="D20" s="15" t="n">
-        <v>658.5</v>
+        <v>620.05</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>659.25</v>
+        <v>619.5</v>
       </c>
       <c r="F20" s="18" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G20" s="6" t="n">
-        <v>666</v>
+        <v>615.55</v>
       </c>
     </row>
     <row r="21">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B21" s="9" t="n">
-        <v>3185.45</v>
+        <v>3188</v>
       </c>
       <c r="C21" s="12" t="n">
-        <v>3111.55</v>
+        <v>3121</v>
       </c>
       <c r="D21" s="15" t="n">
-        <v>3168</v>
+        <v>3136.8</v>
       </c>
       <c r="E21" s="6" t="n">
-        <v>3165.5</v>
+        <v>3134.35</v>
       </c>
       <c r="F21" s="18" t="n">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>3128.7</v>
+        <v>3180.75</v>
       </c>
     </row>
     <row r="22">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B22" s="9" t="n">
-        <v>338.45</v>
+        <v>287.05</v>
       </c>
       <c r="C22" s="12" t="n">
-        <v>328.05</v>
+        <v>282.6</v>
       </c>
       <c r="D22" s="15" t="n">
-        <v>332.55</v>
+        <v>284.4</v>
       </c>
       <c r="E22" s="6" t="n">
-        <v>330.1</v>
+        <v>284.05</v>
       </c>
       <c r="F22" s="18" t="n">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="G22" s="6" t="n">
-        <v>337.75</v>
+        <v>284.45</v>
       </c>
     </row>
     <row r="23">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B23" s="9" t="n">
-        <v>446.55</v>
+        <v>426.65</v>
       </c>
       <c r="C23" s="12" t="n">
-        <v>438.8</v>
+        <v>420.3</v>
       </c>
       <c r="D23" s="15" t="n">
-        <v>440.8</v>
+        <v>422.5</v>
       </c>
       <c r="E23" s="6" t="n">
-        <v>440.1</v>
+        <v>422.5</v>
       </c>
       <c r="F23" s="18" t="n">
-        <v>159</v>
+        <v>86</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>444.6</v>
+        <v>420.6</v>
       </c>
     </row>
     <row r="24">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B24" s="9" t="n">
-        <v>2967.65</v>
+        <v>2766.55</v>
       </c>
       <c r="C24" s="12" t="n">
-        <v>2925.65</v>
+        <v>2740</v>
       </c>
       <c r="D24" s="15" t="n">
-        <v>2927</v>
+        <v>2749</v>
       </c>
       <c r="E24" s="6" t="n">
-        <v>2929.65</v>
+        <v>2744.2</v>
       </c>
       <c r="F24" s="18" t="n">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="G24" s="6" t="n">
-        <v>2967.35</v>
+        <v>2751.95</v>
       </c>
     </row>
     <row r="25">
@@ -1222,22 +1222,22 @@
         </is>
       </c>
       <c r="B25" s="9" t="n">
-        <v>800.35</v>
+        <v>802.7</v>
       </c>
       <c r="C25" s="12" t="n">
-        <v>791.7</v>
+        <v>793</v>
       </c>
       <c r="D25" s="15" t="n">
-        <v>795.5</v>
+        <v>799</v>
       </c>
       <c r="E25" s="6" t="n">
-        <v>796.95</v>
+        <v>799.75</v>
       </c>
       <c r="F25" s="18" t="n">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="G25" s="6" t="n">
-        <v>794.75</v>
+        <v>797</v>
       </c>
     </row>
     <row r="26">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B26" s="9" t="n">
-        <v>853</v>
+        <v>795.65</v>
       </c>
       <c r="C26" s="12" t="n">
-        <v>833.85</v>
+        <v>782</v>
       </c>
       <c r="D26" s="15" t="n">
-        <v>849.3</v>
+        <v>782.45</v>
       </c>
       <c r="E26" s="6" t="n">
-        <v>849.65</v>
+        <v>783.85</v>
       </c>
       <c r="F26" s="18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G26" s="6" t="n">
-        <v>837.5</v>
+        <v>787.05</v>
       </c>
     </row>
     <row r="27">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B27" s="9" t="n">
-        <v>1139.95</v>
+        <v>1188.7</v>
       </c>
       <c r="C27" s="12" t="n">
-        <v>1090.35</v>
+        <v>1152.9</v>
       </c>
       <c r="D27" s="15" t="n">
-        <v>1130.9</v>
+        <v>1183.5</v>
       </c>
       <c r="E27" s="6" t="n">
-        <v>1132.6</v>
+        <v>1183.1</v>
       </c>
       <c r="F27" s="18" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G27" s="6" t="n">
-        <v>1093.8</v>
+        <v>1161.75</v>
       </c>
     </row>
     <row r="28">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B28" s="9" t="n">
-        <v>984.5</v>
+        <v>937</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>958.9</v>
+        <v>928.5</v>
       </c>
       <c r="D28" s="15" t="n">
-        <v>966.4</v>
+        <v>931.4</v>
       </c>
       <c r="E28" s="6" t="n">
-        <v>965.2</v>
+        <v>930.7</v>
       </c>
       <c r="F28" s="18" t="n">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="G28" s="6" t="n">
-        <v>980</v>
+        <v>930.15</v>
       </c>
     </row>
     <row r="29">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B29" s="9" t="n">
-        <v>491.2</v>
+        <v>466.3</v>
       </c>
       <c r="C29" s="12" t="n">
-        <v>479.4</v>
+        <v>459.55</v>
       </c>
       <c r="D29" s="15" t="n">
-        <v>481</v>
+        <v>461.5</v>
       </c>
       <c r="E29" s="6" t="n">
-        <v>481.25</v>
+        <v>461.15</v>
       </c>
       <c r="F29" s="18" t="n">
-        <v>151</v>
+        <v>80</v>
       </c>
       <c r="G29" s="6" t="n">
-        <v>486.7</v>
+        <v>462.7</v>
       </c>
     </row>
     <row r="30">
@@ -1347,22 +1347,22 @@
         </is>
       </c>
       <c r="B30" s="9" t="n">
-        <v>168.37</v>
+        <v>163.78</v>
       </c>
       <c r="C30" s="12" t="n">
-        <v>165.1</v>
+        <v>160.39</v>
       </c>
       <c r="D30" s="15" t="n">
-        <v>166.7</v>
+        <v>160.85</v>
       </c>
       <c r="E30" s="6" t="n">
-        <v>167.03</v>
+        <v>160.66</v>
       </c>
       <c r="F30" s="18" t="n">
-        <v>507</v>
+        <v>532</v>
       </c>
       <c r="G30" s="6" t="n">
-        <v>168.12</v>
+        <v>160.7</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" thickBot="1">
@@ -1372,22 +1372,22 @@
         </is>
       </c>
       <c r="B31" s="10" t="n">
-        <v>11887.7</v>
+        <v>11468.3</v>
       </c>
       <c r="C31" s="13" t="n">
-        <v>11650.25</v>
+        <v>11377.05</v>
       </c>
       <c r="D31" s="16" t="n">
-        <v>11849.85</v>
+        <v>11423.2</v>
       </c>
       <c r="E31" s="7" t="n">
-        <v>11837.15</v>
+        <v>11421.3</v>
       </c>
       <c r="F31" s="19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G31" s="7" t="n">
-        <v>11798.8</v>
+        <v>11391.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>